<commit_message>
DM-477: update practice editor
</commit_message>
<xml_diff>
--- a/lib/assets/Diffusion_Marketplace.xlsx
+++ b/lib/assets/Diffusion_Marketplace.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2857" uniqueCount="1713">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2856" uniqueCount="1713">
   <si>
     <t xml:space="preserve">Respondent ID</t>
   </si>
@@ -1884,7 +1884,7 @@
     <t xml:space="preserve">Kristina.Cordasco@va.gov</t>
   </si>
   <si>
-    <t xml:space="preserve">kristina.cordasco@va.gov</t>
+    <t xml:space="preserve">VHAWLAEDPACT@va.gov</t>
   </si>
   <si>
     <t xml:space="preserve">The ED-PACT Tool</t>
@@ -2007,19 +2007,19 @@
     <t xml:space="preserve">permanent</t>
   </si>
   <si>
+    <t xml:space="preserve">Clinical Champion; Administrative Assistant/Project Manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 hour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">description of ED-PACT Tool and discussion of 5 cases, review of RN Care Manager guide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
     <t xml:space="preserve">none</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clinical Champion; Administrative Assistant/Project Manager</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 hour</t>
-  </si>
-  <si>
-    <t xml:space="preserve">description of ED-PACT Tool and discussion of 5 cases, review of RN Care Manager guide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no</t>
   </si>
   <si>
     <t xml:space="preserve">ED Director Permission</t>
@@ -5358,7 +5358,7 @@
   <dimension ref="A1:MT27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8618,7 +8618,7 @@
         <v>43603.4922106482</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>43622.6010648148</v>
+        <v>43668.3460416667</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>618</v>
@@ -8797,26 +8797,23 @@
       <c r="CB9" s="0" t="s">
         <v>660</v>
       </c>
-      <c r="CC9" s="0" t="s">
+      <c r="CH9" s="0" t="s">
         <v>661</v>
-      </c>
-      <c r="CH9" s="0" t="s">
-        <v>662</v>
       </c>
       <c r="CI9" s="0" t="s">
         <v>653</v>
       </c>
       <c r="CN9" s="0" t="s">
+        <v>662</v>
+      </c>
+      <c r="CO9" s="0" t="s">
         <v>663</v>
       </c>
-      <c r="CO9" s="0" t="s">
+      <c r="CP9" s="0" t="s">
         <v>664</v>
       </c>
-      <c r="CP9" s="0" t="s">
+      <c r="CQ9" s="0" t="s">
         <v>665</v>
-      </c>
-      <c r="CQ9" s="0" t="s">
-        <v>661</v>
       </c>
       <c r="CW9" s="0" t="s">
         <v>365</v>
@@ -11241,7 +11238,7 @@
         <v>1088</v>
       </c>
       <c r="CP17" s="0" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="CQ17" s="0" t="s">
         <v>1083</v>
@@ -11881,7 +11878,7 @@
         <v>1207</v>
       </c>
       <c r="CP19" s="0" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="CW19" s="0" t="s">
         <v>365</v>
@@ -12243,7 +12240,7 @@
         <v>1279</v>
       </c>
       <c r="CN20" s="0" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="CO20" s="0" t="s">
         <v>1280</v>
@@ -13317,7 +13314,7 @@
         <v>1466</v>
       </c>
       <c r="CP23" s="0" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="CQ23" s="0" t="s">
         <v>1467</v>

</xml_diff>

<commit_message>
DM-477: update practice editor (#79)
* DM-UPGRADE: upgrade ruby to 2.6.3

* DM-UPGRADE: upgrade tests to use bundler 2

* DM-UPGRADE: upgrade tests to use bundler 2

* DM-477: update practice editor
</commit_message>
<xml_diff>
--- a/lib/assets/Diffusion_Marketplace.xlsx
+++ b/lib/assets/Diffusion_Marketplace.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2857" uniqueCount="1713">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2856" uniqueCount="1713">
   <si>
     <t xml:space="preserve">Respondent ID</t>
   </si>
@@ -1884,7 +1884,7 @@
     <t xml:space="preserve">Kristina.Cordasco@va.gov</t>
   </si>
   <si>
-    <t xml:space="preserve">kristina.cordasco@va.gov</t>
+    <t xml:space="preserve">VHAWLAEDPACT@va.gov</t>
   </si>
   <si>
     <t xml:space="preserve">The ED-PACT Tool</t>
@@ -2007,19 +2007,19 @@
     <t xml:space="preserve">permanent</t>
   </si>
   <si>
+    <t xml:space="preserve">Clinical Champion; Administrative Assistant/Project Manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 hour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">description of ED-PACT Tool and discussion of 5 cases, review of RN Care Manager guide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
     <t xml:space="preserve">none</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clinical Champion; Administrative Assistant/Project Manager</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 hour</t>
-  </si>
-  <si>
-    <t xml:space="preserve">description of ED-PACT Tool and discussion of 5 cases, review of RN Care Manager guide</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no</t>
   </si>
   <si>
     <t xml:space="preserve">ED Director Permission</t>
@@ -5358,7 +5358,7 @@
   <dimension ref="A1:MT27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8618,7 +8618,7 @@
         <v>43603.4922106482</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>43622.6010648148</v>
+        <v>43668.3460416667</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>618</v>
@@ -8797,26 +8797,23 @@
       <c r="CB9" s="0" t="s">
         <v>660</v>
       </c>
-      <c r="CC9" s="0" t="s">
+      <c r="CH9" s="0" t="s">
         <v>661</v>
-      </c>
-      <c r="CH9" s="0" t="s">
-        <v>662</v>
       </c>
       <c r="CI9" s="0" t="s">
         <v>653</v>
       </c>
       <c r="CN9" s="0" t="s">
+        <v>662</v>
+      </c>
+      <c r="CO9" s="0" t="s">
         <v>663</v>
       </c>
-      <c r="CO9" s="0" t="s">
+      <c r="CP9" s="0" t="s">
         <v>664</v>
       </c>
-      <c r="CP9" s="0" t="s">
+      <c r="CQ9" s="0" t="s">
         <v>665</v>
-      </c>
-      <c r="CQ9" s="0" t="s">
-        <v>661</v>
       </c>
       <c r="CW9" s="0" t="s">
         <v>365</v>
@@ -11241,7 +11238,7 @@
         <v>1088</v>
       </c>
       <c r="CP17" s="0" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="CQ17" s="0" t="s">
         <v>1083</v>
@@ -11881,7 +11878,7 @@
         <v>1207</v>
       </c>
       <c r="CP19" s="0" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="CW19" s="0" t="s">
         <v>365</v>
@@ -12243,7 +12240,7 @@
         <v>1279</v>
       </c>
       <c r="CN20" s="0" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="CO20" s="0" t="s">
         <v>1280</v>
@@ -13317,7 +13314,7 @@
         <v>1466</v>
       </c>
       <c r="CP23" s="0" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="CQ23" s="0" t="s">
         <v>1467</v>

</xml_diff>

<commit_message>
DM-1110 Confirmation page update
</commit_message>
<xml_diff>
--- a/lib/assets/Diffusion_Marketplace.xlsx
+++ b/lib/assets/Diffusion_Marketplace.xlsx
@@ -7921,7 +7921,7 @@
         <v>43734.60157407408</v>
       </c>
       <c r="D15" s="1">
-        <v>43753.32494212963</v>
+        <v>43754.683333333334</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -8382,6 +8382,11 @@
           <t>17-minute video developed by VA Employee Education System (EES). VA subject matter experts for tinnitus worked with EES staff to create and produce this video. It is intended as a general information video for Veterans to ensure them that good help is available for tinnitus using the VA-endorsed method of Progressive Tinnitus Management (PTM). The first approximately 12 minutes show an entertaining and informative skit of a younger and older Veteran addressing the younger Veteran’s tinnitus. The remaining 5 minutes are an explanation of tinnitus by a VA audiologist as well as a description of PTM. </t>
         </is>
       </c>
+      <c r="MG15" t="inlineStr">
+        <is>
+          <t>Item 67 combined docs.pdf</t>
+        </is>
+      </c>
       <c r="MH15" t="inlineStr">
         <is>
           <t>Item 68 Links to PTM resources.pdf</t>
@@ -8389,7 +8394,7 @@
       </c>
       <c r="MM15" t="inlineStr">
         <is>
-          <t>Item 73 Peer reviewed article 2.pdf</t>
+          <t>Item 73 combined docs.pdf</t>
         </is>
       </c>
       <c r="MN15" t="inlineStr">
@@ -10404,7 +10409,7 @@
         <v>43713.234456018516</v>
       </c>
       <c r="D20" s="1">
-        <v>43739.343125</v>
+        <v>43755.35863425926</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -10438,7 +10443,7 @@
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>With our teleRehabilitation wheeled mobility clinic, we partnered with our contract nursing home facilities to complete complex wheelchair seating assessments and deliver equipment to our Veterans without the need for travel to a VA facility. Using telehealth technology, rehab clinicians work together with the community therapists to evaluate, measure, fit, train and deliver a specialized wheelchair over the course of multiple visits. Vendors are used to assist with delivery of the equipment and provide hands on assist with set up of the wheelchair. Using telerehabilitation has enabled Veterans to get the care they need, eliminating hardships with travel to the VA. </t>
+          <t>With our TeleRehabilitation wheeled mobility clinic, we partnered with our contract nursing home facilities to complete complex wheelchair seating assessments and deliver equipment to our Veterans without the need for travel to a VA facility. Using telehealth technology, rehab clinicians work together with the community therapists to evaluate, measure, fit, train and deliver a specialized wheelchair over the course of multiple visits. Vendors are used to assist with delivery of the equipment and provide hands on assist with set up of the wheelchair. Using telerehabilitation has enabled Veterans to get the care they need, eliminating hardships with travel to the VA. </t>
         </is>
       </c>
       <c r="O20" t="inlineStr">
@@ -10468,7 +10473,7 @@
       </c>
       <c r="U20" t="inlineStr">
         <is>
-          <t>VHA_618</t>
+          <t>vha_618</t>
         </is>
       </c>
       <c r="V20" t="inlineStr">
@@ -10489,7 +10494,7 @@
       </c>
       <c r="AA20" t="inlineStr">
         <is>
-          <t>Identify your team: PT/OT/CNH Coordinator</t>
+          <t>Identify your team: PT/OT/CNH (Community Nursing Home) Coordinator</t>
         </is>
       </c>
       <c r="AB20" t="inlineStr">
@@ -10509,7 +10514,7 @@
       </c>
       <c r="AE20" t="inlineStr">
         <is>
-          <t>Complete telehealth training/requirements (VA Staff, CNH, vendors)</t>
+          <t>Complete telehealth training/requirements (VA Staff, Community Nursing Home, vendors)</t>
         </is>
       </c>
       <c r="AF20" t="inlineStr">
@@ -10559,12 +10564,37 @@
       </c>
       <c r="BC20" t="inlineStr">
         <is>
-          <t>dddgadgdg</t>
+          <t>CNH (Community Nursing Home) liaison </t>
+        </is>
+      </c>
+      <c r="BD20" t="inlineStr">
+        <is>
+          <t>Identify alternative coodinator role</t>
+        </is>
+      </c>
+      <c r="BE20" t="inlineStr">
+        <is>
+          <t>Clinicians lack specialized training to initiate </t>
+        </is>
+      </c>
+      <c r="BF20" t="inlineStr">
+        <is>
+          <t>Identify other clinicians available via telehealth, or provide funds for training</t>
+        </is>
+      </c>
+      <c r="BG20" t="inlineStr">
+        <is>
+          <t>CNH willingness to participate</t>
+        </is>
+      </c>
+      <c r="BH20" t="inlineStr">
+        <is>
+          <t>Education, marketing, training, benefits</t>
         </is>
       </c>
       <c r="BI20" t="inlineStr">
         <is>
-          <t>2. $10,000 - $50,000</t>
+          <t>3. $50,000 - $250,000</t>
         </is>
       </c>
       <c r="BJ20" t="inlineStr">
@@ -10584,22 +10614,142 @@
       </c>
       <c r="BM20" t="inlineStr">
         <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BN20" t="inlineStr">
+        <is>
+          <t>New Clinical Approach or New Process</t>
+        </is>
+      </c>
+      <c r="BO20" t="inlineStr">
+        <is>
+          <t>Coordinator</t>
+        </is>
+      </c>
+      <c r="BP20" t="inlineStr">
+        <is>
+          <t>Physical Therapist</t>
+        </is>
+      </c>
+      <c r="BQ20" t="inlineStr">
+        <is>
+          <t>Occupational Therapist</t>
+        </is>
+      </c>
+      <c r="BR20" t="inlineStr">
+        <is>
+          <t>MSA ( Medical Support Assistant) </t>
+        </is>
+      </c>
+      <c r="BT20" t="inlineStr">
+        <is>
+          <t>1 hr</t>
+        </is>
+      </c>
+      <c r="BU20" t="inlineStr">
+        <is>
+          <t>4 hrs</t>
+        </is>
+      </c>
+      <c r="BV20" t="inlineStr">
+        <is>
+          <t>4 hrs</t>
+        </is>
+      </c>
+      <c r="BW20" t="inlineStr">
+        <is>
+          <t>&gt;1 hr</t>
+        </is>
+      </c>
+      <c r="BY20" t="inlineStr">
+        <is>
+          <t>Permanent</t>
+        </is>
+      </c>
+      <c r="BZ20" t="inlineStr">
+        <is>
+          <t>Permanent</t>
+        </is>
+      </c>
+      <c r="CA20" t="inlineStr">
+        <is>
+          <t>Permanent</t>
+        </is>
+      </c>
+      <c r="CB20" t="inlineStr">
+        <is>
+          <t>Permanent</t>
+        </is>
+      </c>
+      <c r="CD20" t="inlineStr">
+        <is>
+          <t>I Pad, or TeleHealth Computer </t>
+        </is>
+      </c>
+      <c r="CE20" t="inlineStr">
+        <is>
+          <t>Space for Telehealth computer and meeting</t>
+        </is>
+      </c>
+      <c r="CF20" t="inlineStr">
+        <is>
+          <t>Camera</t>
+        </is>
+      </c>
+      <c r="CI20" t="inlineStr">
+        <is>
+          <t>TeleRehab Program Manager/CNH Coordinator</t>
+        </is>
+      </c>
+      <c r="CJ20" t="inlineStr">
+        <is>
+          <t>Coordinator/Staff</t>
+        </is>
+      </c>
+      <c r="CK20" t="inlineStr">
+        <is>
+          <t>Physical Therapist</t>
+        </is>
+      </c>
+      <c r="CL20" t="inlineStr">
+        <is>
+          <t>Occupational Therapist</t>
+        </is>
+      </c>
+      <c r="CM20" t="inlineStr">
+        <is>
+          <t>Occupational Therapist</t>
+        </is>
+      </c>
+      <c r="CN20" t="inlineStr">
+        <is>
+          <t>MD assigned to CNH</t>
+        </is>
+      </c>
+      <c r="CO20" t="inlineStr">
+        <is>
+          <t>60 min</t>
+        </is>
+      </c>
+      <c r="CP20" t="inlineStr">
+        <is>
+          <t>SOP and Telehealth Training TMS</t>
+        </is>
+      </c>
+      <c r="CQ20" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="BN20" t="inlineStr">
-        <is>
-          <t>Modification of an established process</t>
-        </is>
-      </c>
-      <c r="CD20" t="inlineStr">
-        <is>
-          <t>I Pad , or Tele Health Computer </t>
-        </is>
-      </c>
-      <c r="CE20" t="inlineStr">
-        <is>
-          <t>Space for telehealth computer and meeting</t>
+      <c r="CR20" t="inlineStr">
+        <is>
+          <t>Prosthetic funding to pay vendor</t>
+        </is>
+      </c>
+      <c r="CS20" t="inlineStr">
+        <is>
+          <t>CNH program pays community therapists' time</t>
         </is>
       </c>
       <c r="CX20" t="inlineStr">
@@ -10607,6 +10757,76 @@
           <t>No</t>
         </is>
       </c>
+      <c r="CY20" t="inlineStr">
+        <is>
+          <t>CNH contract</t>
+        </is>
+      </c>
+      <c r="DD20" t="inlineStr">
+        <is>
+          <t>Grace Wilske150x150.jpg</t>
+        </is>
+      </c>
+      <c r="DE20" t="inlineStr">
+        <is>
+          <t>TeleRehab tasked to create Wheeled Mobility clinic</t>
+        </is>
+      </c>
+      <c r="DF20" t="inlineStr">
+        <is>
+          <t>In 2017, the Office of Rural Health funded the TeleRehabilitation Enterprise Wide Initiative. Many telehealth protocols were created, and our teams were tasked to innovate a practice to provide wheeled mobility services to Veterans via telehealth. Many ideas were generated to build a successful clinic, but there were difficulties and barriers along the way as we needed support where the Veteran was located. Once we met with our CNH director, we knew we had found a collaborative approach to connect our Veterans in the CNH to our specialized services. This has been the bridge for a successful partnership!</t>
+        </is>
+      </c>
+      <c r="DG20" t="inlineStr">
+        <is>
+          <t>Impact1CNH696x392.jpg</t>
+        </is>
+      </c>
+      <c r="DH20" t="inlineStr">
+        <is>
+          <t>Wheelchair Telerehab to the Community Nursing Home</t>
+        </is>
+      </c>
+      <c r="DI20" t="inlineStr">
+        <is>
+          <t>Through telerehab visits, our VA Occupational Therapist guides the community therapist with adjustments or modifications. We provide education to the functionality of the power wheelchair issued to the Veteran. The community therapist helps facilitate through their eyes, hands, and skills. </t>
+        </is>
+      </c>
+      <c r="DJ20" t="inlineStr">
+        <is>
+          <t>Impact2VAOTvideoclinic696x392.jpg</t>
+        </is>
+      </c>
+      <c r="DK20" t="inlineStr">
+        <is>
+          <t>VA Therapist conducts WC evaluation</t>
+        </is>
+      </c>
+      <c r="DL20" t="inlineStr">
+        <is>
+          <t>Through telerehab visits, our VA therapist instructs the community therapist in measuring for a custom fit. The Veteran may trial different wheelchairs in their home environment for optimal use. </t>
+        </is>
+      </c>
+      <c r="DM20" t="inlineStr">
+        <is>
+          <t>Impact3CoordinatorTestCall 696x392.jpg</t>
+        </is>
+      </c>
+      <c r="DN20" t="inlineStr">
+        <is>
+          <t>Coordinator completing test call with CNH</t>
+        </is>
+      </c>
+      <c r="DO20" t="inlineStr">
+        <is>
+          <t>Our CNH coordinator completes a test call with the therapist at the CNH, to ensure good technology connection during the visit. Details about the visit are provided and a welcome letter is sent with instructions. </t>
+        </is>
+      </c>
+      <c r="DP20" t="inlineStr">
+        <is>
+          <t>VHAMINTREWIWC@va.gov</t>
+        </is>
+      </c>
       <c r="DQ20" t="inlineStr">
         <is>
           <t>Grace Wilske\TeleRehab Program Manager, Occupational Therapist </t>
@@ -10627,6 +10847,36 @@
           <t> Benjamin Barrett\Occupational Therapist </t>
         </is>
       </c>
+      <c r="DU20" t="inlineStr">
+        <is>
+          <t>Dr. Larisa Kusar\MD,Dr. Mary Matsumoto\MD,Taylor Nelson, Lead MSA,Tad Nielsen, OTR/L, ATP</t>
+        </is>
+      </c>
+      <c r="DV20" t="inlineStr">
+        <is>
+          <t>Grace Wilske65x65(1).jpg</t>
+        </is>
+      </c>
+      <c r="DW20" t="inlineStr">
+        <is>
+          <t>Jessica Hollie65x65.jpg</t>
+        </is>
+      </c>
+      <c r="DX20" t="inlineStr">
+        <is>
+          <t>Kristin Hanowski65x65.jpg</t>
+        </is>
+      </c>
+      <c r="DY20" t="inlineStr">
+        <is>
+          <t>Benjamin Barrett65x65.jpg</t>
+        </is>
+      </c>
+      <c r="DZ20" t="inlineStr">
+        <is>
+          <t>Teamsupport65x65.jpg</t>
+        </is>
+      </c>
       <c r="EA20" t="inlineStr">
         <is>
           <t>Veteran - Enables an improvement in satisfaction or customer experience for Veterans</t>
@@ -10677,9 +10927,29 @@
           <t>All primary care specialties equally - not a search differentiator</t>
         </is>
       </c>
-      <c r="GT20" t="inlineStr">
-        <is>
-          <t>All medical sub-specialties equally - not a search differentiator</t>
+      <c r="GN20" t="inlineStr">
+        <is>
+          <t>Rehab Medicine</t>
+        </is>
+      </c>
+      <c r="GQ20" t="inlineStr">
+        <is>
+          <t>Specialty Care (outside of VA)</t>
+        </is>
+      </c>
+      <c r="HB20" t="inlineStr">
+        <is>
+          <t>Orthopedic Surgery</t>
+        </is>
+      </c>
+      <c r="HD20" t="inlineStr">
+        <is>
+          <t>Specialty Care (outside of VA)</t>
+        </is>
+      </c>
+      <c r="HF20" t="inlineStr">
+        <is>
+          <t>Trauma Surgery</t>
         </is>
       </c>
       <c r="HI20" t="inlineStr">
@@ -10692,9 +10962,99 @@
           <t>Complementary Therapies</t>
         </is>
       </c>
-      <c r="JF20" t="inlineStr">
-        <is>
-          <t>All clinical conditions equally - not a search differentiator</t>
+      <c r="HS20" t="inlineStr">
+        <is>
+          <t>Parkinson's disease</t>
+        </is>
+      </c>
+      <c r="HT20" t="inlineStr">
+        <is>
+          <t>Wheelchair dependent</t>
+        </is>
+      </c>
+      <c r="HU20" t="inlineStr">
+        <is>
+          <t>SCI (Spinal Cord Injury)</t>
+        </is>
+      </c>
+      <c r="HV20" t="inlineStr">
+        <is>
+          <t>Amputation</t>
+        </is>
+      </c>
+      <c r="HW20" t="inlineStr">
+        <is>
+          <t>Failure to thrive</t>
+        </is>
+      </c>
+      <c r="HX20" t="inlineStr">
+        <is>
+          <t>Neurology</t>
+        </is>
+      </c>
+      <c r="HZ20" t="inlineStr">
+        <is>
+          <t>Stroke</t>
+        </is>
+      </c>
+      <c r="IB20" t="inlineStr">
+        <is>
+          <t>Trauma</t>
+        </is>
+      </c>
+      <c r="IE20" t="inlineStr">
+        <is>
+          <t>Infection</t>
+        </is>
+      </c>
+      <c r="IF20" t="inlineStr">
+        <is>
+          <t>Cardiovascular</t>
+        </is>
+      </c>
+      <c r="IG20" t="inlineStr">
+        <is>
+          <t>Congestive heart failure (CHF)</t>
+        </is>
+      </c>
+      <c r="IJ20" t="inlineStr">
+        <is>
+          <t>Pulmonary</t>
+        </is>
+      </c>
+      <c r="IK20" t="inlineStr">
+        <is>
+          <t>Chronic Obstructive Pulmonary Disease (COPD)</t>
+        </is>
+      </c>
+      <c r="IQ20" t="inlineStr">
+        <is>
+          <t>Obesity</t>
+        </is>
+      </c>
+      <c r="IT20" t="inlineStr">
+        <is>
+          <t>Pelvis</t>
+        </is>
+      </c>
+      <c r="IU20" t="inlineStr">
+        <is>
+          <t>Extremities</t>
+        </is>
+      </c>
+      <c r="IV20" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="IW20" t="inlineStr">
+        <is>
+          <t>Whole body</t>
+        </is>
+      </c>
+      <c r="IZ20" t="inlineStr">
+        <is>
+          <t>Trauma</t>
         </is>
       </c>
       <c r="JJ20" t="inlineStr">
@@ -10717,6 +11077,16 @@
           <t>Social Work</t>
         </is>
       </c>
+      <c r="KD20" t="inlineStr">
+        <is>
+          <t>Discharge Planning</t>
+        </is>
+      </c>
+      <c r="KE20" t="inlineStr">
+        <is>
+          <t>Education and Training</t>
+        </is>
+      </c>
       <c r="KF20" t="inlineStr">
         <is>
           <t>Elderly Services</t>
@@ -10737,9 +11107,39 @@
           <t>Occupational Health and Safety</t>
         </is>
       </c>
-      <c r="MA20" t="inlineStr">
-        <is>
-          <t>All job titles equally - not a search differentiator</t>
+      <c r="LS20" t="inlineStr">
+        <is>
+          <t>Clinic based physician</t>
+        </is>
+      </c>
+      <c r="MB20" t="inlineStr">
+        <is>
+          <t>Community based therapy</t>
+        </is>
+      </c>
+      <c r="MC20" t="inlineStr">
+        <is>
+          <t>Tele rehab 384x216.jpg</t>
+        </is>
+      </c>
+      <c r="ME20" t="inlineStr">
+        <is>
+          <t>Telerehab makes Veterans lives easier</t>
+        </is>
+      </c>
+      <c r="MF20" t="inlineStr">
+        <is>
+          <t>Using Telerehab wheeled mobility clinics. Veterans receive care by bridging the gap for rural access to rehabilitation services. </t>
+        </is>
+      </c>
+      <c r="ML20" t="inlineStr">
+        <is>
+          <t>https://www.vapulse.net/groups/trewi-telerehabilitation-enterprise-wide-initiative</t>
+        </is>
+      </c>
+      <c r="MU20" t="inlineStr">
+        <is>
+          <t>Clarifying implementation of new practice vs new practice in motion</t>
         </is>
       </c>
     </row>
@@ -12233,7 +12633,7 @@
         <v>43705.50811342592</v>
       </c>
       <c r="D24" s="1">
-        <v>43746.34297453704</v>
+        <v>43754.741944444446</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -12257,12 +12657,12 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>On demand tele-geropsychiatry consultation through tele-health. </t>
+          <t>On demand tele-geropsychiatry consultation through telehealth. </t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>Provide rapid consultation on geropsychiatry issues to Veterans across VISN 23. Platforms include tele-health (VA video connect to home, clinical video telehealth) e-consultation and team meetings as requested. </t>
+          <t>Provide rapid consultation on geropsychiatry issues to Veterans across VISN 23. Platforms include telehealth (VA video connect to home, clinical video telehealth) e-consultation and team meetings as requested. </t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
@@ -12297,7 +12697,7 @@
       </c>
       <c r="U24" t="inlineStr">
         <is>
-          <t>VISN23</t>
+          <t>vha_VISN23</t>
         </is>
       </c>
       <c r="V24" t="inlineStr">
@@ -12446,51 +12846,43 @@
           <t>Assoc. Director of tele-mental health </t>
         </is>
       </c>
-      <c r="BT24" t="inlineStr">
+      <c r="BT24">
+        <v>40</v>
+      </c>
+      <c r="BU24">
+        <v>20</v>
+      </c>
+      <c r="BV24" t="inlineStr">
+        <is>
+          <t>5 to 7</t>
+        </is>
+      </c>
+      <c r="BW24">
+        <v>2</v>
+      </c>
+      <c r="BX24">
+        <v>1</v>
+      </c>
+      <c r="BY24" t="inlineStr">
         <is>
           <t>Permanent</t>
         </is>
       </c>
-      <c r="BU24" t="inlineStr">
+      <c r="BZ24" t="inlineStr">
         <is>
           <t>Permanent</t>
         </is>
       </c>
-      <c r="BV24" t="inlineStr">
-        <is>
-          <t>Permanent</t>
-        </is>
-      </c>
-      <c r="BW24" t="inlineStr">
-        <is>
-          <t>Permanent</t>
-        </is>
-      </c>
-      <c r="BX24" t="inlineStr">
-        <is>
-          <t>Permanent</t>
-        </is>
-      </c>
-      <c r="BY24" t="inlineStr">
-        <is>
-          <t>Tele-health equipment. (All tele-health staff on Hub side and pt side).</t>
-        </is>
-      </c>
-      <c r="BZ24" t="inlineStr">
+      <c r="CD24" t="inlineStr">
+        <is>
+          <t>Telehealth equipment. (All tele-health staff on Hub side and pt side).</t>
+        </is>
+      </c>
+      <c r="CE24" t="inlineStr">
         <is>
           <t>Dx, ipads, computers, phone, etc. </t>
         </is>
       </c>
-      <c r="CD24" t="inlineStr">
-        <is>
-          <t>Tele-health equipment. (All tele-health staff on Hub side and pt side).</t>
-        </is>
-      </c>
-      <c r="CE24" t="inlineStr">
-        <is>
-          <t>Dx, ipads, computers, phone, etc. </t>
-        </is>
-      </c>
       <c r="CI24" t="inlineStr">
         <is>
           <t>For Hub employees are trained by Hub. Spoke sites are trained by Spoke FTC</t>
@@ -12528,12 +12920,12 @@
       </c>
       <c r="CY24" t="inlineStr">
         <is>
-          <t>MOU</t>
+          <t>MOU  (Memorandum of Understanding)</t>
         </is>
       </c>
       <c r="CZ24" t="inlineStr">
         <is>
-          <t>TSA</t>
+          <t>TSA  (Telehealth service agreement)</t>
         </is>
       </c>
       <c r="DD24" t="inlineStr">
@@ -12553,12 +12945,22 @@
       </c>
       <c r="DG24" t="inlineStr">
         <is>
-          <t>696x392 placeholder(1).jpg</t>
+          <t>impactHoldrege_696x392.jpg</t>
         </is>
       </c>
       <c r="DH24" t="inlineStr">
         <is>
-          <t>Innovation in Action</t>
+          <t>Innovative Specialty Care in Action-Reaching Veterans in Rural Clinics or in Their Own Homes</t>
+        </is>
+      </c>
+      <c r="DI24" t="inlineStr">
+        <is>
+          <t>Veterans in the rural Heartland are typically several miles from the nearest medical center, be it private or VA. Travel for the older veteran is also complicated by the his/her own physical limitations including inability to drive. By providing geriatric specialty care via telehealth this vulnerable population has timely access to specialty medicine when the need is recognized.</t>
+        </is>
+      </c>
+      <c r="DJ24" t="inlineStr">
+        <is>
+          <t>house696x392.jpg</t>
         </is>
       </c>
       <c r="DP24" t="inlineStr">

</xml_diff>

<commit_message>
DM-1110 Confirmation page update (#110)
* DM-1110 Confirmation page update

* Fix spec

* Remove focus
</commit_message>
<xml_diff>
--- a/lib/assets/Diffusion_Marketplace.xlsx
+++ b/lib/assets/Diffusion_Marketplace.xlsx
@@ -7921,7 +7921,7 @@
         <v>43734.60157407408</v>
       </c>
       <c r="D15" s="1">
-        <v>43753.32494212963</v>
+        <v>43754.683333333334</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -8382,6 +8382,11 @@
           <t>17-minute video developed by VA Employee Education System (EES). VA subject matter experts for tinnitus worked with EES staff to create and produce this video. It is intended as a general information video for Veterans to ensure them that good help is available for tinnitus using the VA-endorsed method of Progressive Tinnitus Management (PTM). The first approximately 12 minutes show an entertaining and informative skit of a younger and older Veteran addressing the younger Veteran’s tinnitus. The remaining 5 minutes are an explanation of tinnitus by a VA audiologist as well as a description of PTM. </t>
         </is>
       </c>
+      <c r="MG15" t="inlineStr">
+        <is>
+          <t>Item 67 combined docs.pdf</t>
+        </is>
+      </c>
       <c r="MH15" t="inlineStr">
         <is>
           <t>Item 68 Links to PTM resources.pdf</t>
@@ -8389,7 +8394,7 @@
       </c>
       <c r="MM15" t="inlineStr">
         <is>
-          <t>Item 73 Peer reviewed article 2.pdf</t>
+          <t>Item 73 combined docs.pdf</t>
         </is>
       </c>
       <c r="MN15" t="inlineStr">
@@ -10404,7 +10409,7 @@
         <v>43713.234456018516</v>
       </c>
       <c r="D20" s="1">
-        <v>43739.343125</v>
+        <v>43755.35863425926</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -10438,7 +10443,7 @@
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>With our teleRehabilitation wheeled mobility clinic, we partnered with our contract nursing home facilities to complete complex wheelchair seating assessments and deliver equipment to our Veterans without the need for travel to a VA facility. Using telehealth technology, rehab clinicians work together with the community therapists to evaluate, measure, fit, train and deliver a specialized wheelchair over the course of multiple visits. Vendors are used to assist with delivery of the equipment and provide hands on assist with set up of the wheelchair. Using telerehabilitation has enabled Veterans to get the care they need, eliminating hardships with travel to the VA. </t>
+          <t>With our TeleRehabilitation wheeled mobility clinic, we partnered with our contract nursing home facilities to complete complex wheelchair seating assessments and deliver equipment to our Veterans without the need for travel to a VA facility. Using telehealth technology, rehab clinicians work together with the community therapists to evaluate, measure, fit, train and deliver a specialized wheelchair over the course of multiple visits. Vendors are used to assist with delivery of the equipment and provide hands on assist with set up of the wheelchair. Using telerehabilitation has enabled Veterans to get the care they need, eliminating hardships with travel to the VA. </t>
         </is>
       </c>
       <c r="O20" t="inlineStr">
@@ -10468,7 +10473,7 @@
       </c>
       <c r="U20" t="inlineStr">
         <is>
-          <t>VHA_618</t>
+          <t>vha_618</t>
         </is>
       </c>
       <c r="V20" t="inlineStr">
@@ -10489,7 +10494,7 @@
       </c>
       <c r="AA20" t="inlineStr">
         <is>
-          <t>Identify your team: PT/OT/CNH Coordinator</t>
+          <t>Identify your team: PT/OT/CNH (Community Nursing Home) Coordinator</t>
         </is>
       </c>
       <c r="AB20" t="inlineStr">
@@ -10509,7 +10514,7 @@
       </c>
       <c r="AE20" t="inlineStr">
         <is>
-          <t>Complete telehealth training/requirements (VA Staff, CNH, vendors)</t>
+          <t>Complete telehealth training/requirements (VA Staff, Community Nursing Home, vendors)</t>
         </is>
       </c>
       <c r="AF20" t="inlineStr">
@@ -10559,12 +10564,37 @@
       </c>
       <c r="BC20" t="inlineStr">
         <is>
-          <t>dddgadgdg</t>
+          <t>CNH (Community Nursing Home) liaison </t>
+        </is>
+      </c>
+      <c r="BD20" t="inlineStr">
+        <is>
+          <t>Identify alternative coodinator role</t>
+        </is>
+      </c>
+      <c r="BE20" t="inlineStr">
+        <is>
+          <t>Clinicians lack specialized training to initiate </t>
+        </is>
+      </c>
+      <c r="BF20" t="inlineStr">
+        <is>
+          <t>Identify other clinicians available via telehealth, or provide funds for training</t>
+        </is>
+      </c>
+      <c r="BG20" t="inlineStr">
+        <is>
+          <t>CNH willingness to participate</t>
+        </is>
+      </c>
+      <c r="BH20" t="inlineStr">
+        <is>
+          <t>Education, marketing, training, benefits</t>
         </is>
       </c>
       <c r="BI20" t="inlineStr">
         <is>
-          <t>2. $10,000 - $50,000</t>
+          <t>3. $50,000 - $250,000</t>
         </is>
       </c>
       <c r="BJ20" t="inlineStr">
@@ -10584,22 +10614,142 @@
       </c>
       <c r="BM20" t="inlineStr">
         <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BN20" t="inlineStr">
+        <is>
+          <t>New Clinical Approach or New Process</t>
+        </is>
+      </c>
+      <c r="BO20" t="inlineStr">
+        <is>
+          <t>Coordinator</t>
+        </is>
+      </c>
+      <c r="BP20" t="inlineStr">
+        <is>
+          <t>Physical Therapist</t>
+        </is>
+      </c>
+      <c r="BQ20" t="inlineStr">
+        <is>
+          <t>Occupational Therapist</t>
+        </is>
+      </c>
+      <c r="BR20" t="inlineStr">
+        <is>
+          <t>MSA ( Medical Support Assistant) </t>
+        </is>
+      </c>
+      <c r="BT20" t="inlineStr">
+        <is>
+          <t>1 hr</t>
+        </is>
+      </c>
+      <c r="BU20" t="inlineStr">
+        <is>
+          <t>4 hrs</t>
+        </is>
+      </c>
+      <c r="BV20" t="inlineStr">
+        <is>
+          <t>4 hrs</t>
+        </is>
+      </c>
+      <c r="BW20" t="inlineStr">
+        <is>
+          <t>&gt;1 hr</t>
+        </is>
+      </c>
+      <c r="BY20" t="inlineStr">
+        <is>
+          <t>Permanent</t>
+        </is>
+      </c>
+      <c r="BZ20" t="inlineStr">
+        <is>
+          <t>Permanent</t>
+        </is>
+      </c>
+      <c r="CA20" t="inlineStr">
+        <is>
+          <t>Permanent</t>
+        </is>
+      </c>
+      <c r="CB20" t="inlineStr">
+        <is>
+          <t>Permanent</t>
+        </is>
+      </c>
+      <c r="CD20" t="inlineStr">
+        <is>
+          <t>I Pad, or TeleHealth Computer </t>
+        </is>
+      </c>
+      <c r="CE20" t="inlineStr">
+        <is>
+          <t>Space for Telehealth computer and meeting</t>
+        </is>
+      </c>
+      <c r="CF20" t="inlineStr">
+        <is>
+          <t>Camera</t>
+        </is>
+      </c>
+      <c r="CI20" t="inlineStr">
+        <is>
+          <t>TeleRehab Program Manager/CNH Coordinator</t>
+        </is>
+      </c>
+      <c r="CJ20" t="inlineStr">
+        <is>
+          <t>Coordinator/Staff</t>
+        </is>
+      </c>
+      <c r="CK20" t="inlineStr">
+        <is>
+          <t>Physical Therapist</t>
+        </is>
+      </c>
+      <c r="CL20" t="inlineStr">
+        <is>
+          <t>Occupational Therapist</t>
+        </is>
+      </c>
+      <c r="CM20" t="inlineStr">
+        <is>
+          <t>Occupational Therapist</t>
+        </is>
+      </c>
+      <c r="CN20" t="inlineStr">
+        <is>
+          <t>MD assigned to CNH</t>
+        </is>
+      </c>
+      <c r="CO20" t="inlineStr">
+        <is>
+          <t>60 min</t>
+        </is>
+      </c>
+      <c r="CP20" t="inlineStr">
+        <is>
+          <t>SOP and Telehealth Training TMS</t>
+        </is>
+      </c>
+      <c r="CQ20" t="inlineStr">
+        <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="BN20" t="inlineStr">
-        <is>
-          <t>Modification of an established process</t>
-        </is>
-      </c>
-      <c r="CD20" t="inlineStr">
-        <is>
-          <t>I Pad , or Tele Health Computer </t>
-        </is>
-      </c>
-      <c r="CE20" t="inlineStr">
-        <is>
-          <t>Space for telehealth computer and meeting</t>
+      <c r="CR20" t="inlineStr">
+        <is>
+          <t>Prosthetic funding to pay vendor</t>
+        </is>
+      </c>
+      <c r="CS20" t="inlineStr">
+        <is>
+          <t>CNH program pays community therapists' time</t>
         </is>
       </c>
       <c r="CX20" t="inlineStr">
@@ -10607,6 +10757,76 @@
           <t>No</t>
         </is>
       </c>
+      <c r="CY20" t="inlineStr">
+        <is>
+          <t>CNH contract</t>
+        </is>
+      </c>
+      <c r="DD20" t="inlineStr">
+        <is>
+          <t>Grace Wilske150x150.jpg</t>
+        </is>
+      </c>
+      <c r="DE20" t="inlineStr">
+        <is>
+          <t>TeleRehab tasked to create Wheeled Mobility clinic</t>
+        </is>
+      </c>
+      <c r="DF20" t="inlineStr">
+        <is>
+          <t>In 2017, the Office of Rural Health funded the TeleRehabilitation Enterprise Wide Initiative. Many telehealth protocols were created, and our teams were tasked to innovate a practice to provide wheeled mobility services to Veterans via telehealth. Many ideas were generated to build a successful clinic, but there were difficulties and barriers along the way as we needed support where the Veteran was located. Once we met with our CNH director, we knew we had found a collaborative approach to connect our Veterans in the CNH to our specialized services. This has been the bridge for a successful partnership!</t>
+        </is>
+      </c>
+      <c r="DG20" t="inlineStr">
+        <is>
+          <t>Impact1CNH696x392.jpg</t>
+        </is>
+      </c>
+      <c r="DH20" t="inlineStr">
+        <is>
+          <t>Wheelchair Telerehab to the Community Nursing Home</t>
+        </is>
+      </c>
+      <c r="DI20" t="inlineStr">
+        <is>
+          <t>Through telerehab visits, our VA Occupational Therapist guides the community therapist with adjustments or modifications. We provide education to the functionality of the power wheelchair issued to the Veteran. The community therapist helps facilitate through their eyes, hands, and skills. </t>
+        </is>
+      </c>
+      <c r="DJ20" t="inlineStr">
+        <is>
+          <t>Impact2VAOTvideoclinic696x392.jpg</t>
+        </is>
+      </c>
+      <c r="DK20" t="inlineStr">
+        <is>
+          <t>VA Therapist conducts WC evaluation</t>
+        </is>
+      </c>
+      <c r="DL20" t="inlineStr">
+        <is>
+          <t>Through telerehab visits, our VA therapist instructs the community therapist in measuring for a custom fit. The Veteran may trial different wheelchairs in their home environment for optimal use. </t>
+        </is>
+      </c>
+      <c r="DM20" t="inlineStr">
+        <is>
+          <t>Impact3CoordinatorTestCall 696x392.jpg</t>
+        </is>
+      </c>
+      <c r="DN20" t="inlineStr">
+        <is>
+          <t>Coordinator completing test call with CNH</t>
+        </is>
+      </c>
+      <c r="DO20" t="inlineStr">
+        <is>
+          <t>Our CNH coordinator completes a test call with the therapist at the CNH, to ensure good technology connection during the visit. Details about the visit are provided and a welcome letter is sent with instructions. </t>
+        </is>
+      </c>
+      <c r="DP20" t="inlineStr">
+        <is>
+          <t>VHAMINTREWIWC@va.gov</t>
+        </is>
+      </c>
       <c r="DQ20" t="inlineStr">
         <is>
           <t>Grace Wilske\TeleRehab Program Manager, Occupational Therapist </t>
@@ -10627,6 +10847,36 @@
           <t> Benjamin Barrett\Occupational Therapist </t>
         </is>
       </c>
+      <c r="DU20" t="inlineStr">
+        <is>
+          <t>Dr. Larisa Kusar\MD,Dr. Mary Matsumoto\MD,Taylor Nelson, Lead MSA,Tad Nielsen, OTR/L, ATP</t>
+        </is>
+      </c>
+      <c r="DV20" t="inlineStr">
+        <is>
+          <t>Grace Wilske65x65(1).jpg</t>
+        </is>
+      </c>
+      <c r="DW20" t="inlineStr">
+        <is>
+          <t>Jessica Hollie65x65.jpg</t>
+        </is>
+      </c>
+      <c r="DX20" t="inlineStr">
+        <is>
+          <t>Kristin Hanowski65x65.jpg</t>
+        </is>
+      </c>
+      <c r="DY20" t="inlineStr">
+        <is>
+          <t>Benjamin Barrett65x65.jpg</t>
+        </is>
+      </c>
+      <c r="DZ20" t="inlineStr">
+        <is>
+          <t>Teamsupport65x65.jpg</t>
+        </is>
+      </c>
       <c r="EA20" t="inlineStr">
         <is>
           <t>Veteran - Enables an improvement in satisfaction or customer experience for Veterans</t>
@@ -10677,9 +10927,29 @@
           <t>All primary care specialties equally - not a search differentiator</t>
         </is>
       </c>
-      <c r="GT20" t="inlineStr">
-        <is>
-          <t>All medical sub-specialties equally - not a search differentiator</t>
+      <c r="GN20" t="inlineStr">
+        <is>
+          <t>Rehab Medicine</t>
+        </is>
+      </c>
+      <c r="GQ20" t="inlineStr">
+        <is>
+          <t>Specialty Care (outside of VA)</t>
+        </is>
+      </c>
+      <c r="HB20" t="inlineStr">
+        <is>
+          <t>Orthopedic Surgery</t>
+        </is>
+      </c>
+      <c r="HD20" t="inlineStr">
+        <is>
+          <t>Specialty Care (outside of VA)</t>
+        </is>
+      </c>
+      <c r="HF20" t="inlineStr">
+        <is>
+          <t>Trauma Surgery</t>
         </is>
       </c>
       <c r="HI20" t="inlineStr">
@@ -10692,9 +10962,99 @@
           <t>Complementary Therapies</t>
         </is>
       </c>
-      <c r="JF20" t="inlineStr">
-        <is>
-          <t>All clinical conditions equally - not a search differentiator</t>
+      <c r="HS20" t="inlineStr">
+        <is>
+          <t>Parkinson's disease</t>
+        </is>
+      </c>
+      <c r="HT20" t="inlineStr">
+        <is>
+          <t>Wheelchair dependent</t>
+        </is>
+      </c>
+      <c r="HU20" t="inlineStr">
+        <is>
+          <t>SCI (Spinal Cord Injury)</t>
+        </is>
+      </c>
+      <c r="HV20" t="inlineStr">
+        <is>
+          <t>Amputation</t>
+        </is>
+      </c>
+      <c r="HW20" t="inlineStr">
+        <is>
+          <t>Failure to thrive</t>
+        </is>
+      </c>
+      <c r="HX20" t="inlineStr">
+        <is>
+          <t>Neurology</t>
+        </is>
+      </c>
+      <c r="HZ20" t="inlineStr">
+        <is>
+          <t>Stroke</t>
+        </is>
+      </c>
+      <c r="IB20" t="inlineStr">
+        <is>
+          <t>Trauma</t>
+        </is>
+      </c>
+      <c r="IE20" t="inlineStr">
+        <is>
+          <t>Infection</t>
+        </is>
+      </c>
+      <c r="IF20" t="inlineStr">
+        <is>
+          <t>Cardiovascular</t>
+        </is>
+      </c>
+      <c r="IG20" t="inlineStr">
+        <is>
+          <t>Congestive heart failure (CHF)</t>
+        </is>
+      </c>
+      <c r="IJ20" t="inlineStr">
+        <is>
+          <t>Pulmonary</t>
+        </is>
+      </c>
+      <c r="IK20" t="inlineStr">
+        <is>
+          <t>Chronic Obstructive Pulmonary Disease (COPD)</t>
+        </is>
+      </c>
+      <c r="IQ20" t="inlineStr">
+        <is>
+          <t>Obesity</t>
+        </is>
+      </c>
+      <c r="IT20" t="inlineStr">
+        <is>
+          <t>Pelvis</t>
+        </is>
+      </c>
+      <c r="IU20" t="inlineStr">
+        <is>
+          <t>Extremities</t>
+        </is>
+      </c>
+      <c r="IV20" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+      <c r="IW20" t="inlineStr">
+        <is>
+          <t>Whole body</t>
+        </is>
+      </c>
+      <c r="IZ20" t="inlineStr">
+        <is>
+          <t>Trauma</t>
         </is>
       </c>
       <c r="JJ20" t="inlineStr">
@@ -10717,6 +11077,16 @@
           <t>Social Work</t>
         </is>
       </c>
+      <c r="KD20" t="inlineStr">
+        <is>
+          <t>Discharge Planning</t>
+        </is>
+      </c>
+      <c r="KE20" t="inlineStr">
+        <is>
+          <t>Education and Training</t>
+        </is>
+      </c>
       <c r="KF20" t="inlineStr">
         <is>
           <t>Elderly Services</t>
@@ -10737,9 +11107,39 @@
           <t>Occupational Health and Safety</t>
         </is>
       </c>
-      <c r="MA20" t="inlineStr">
-        <is>
-          <t>All job titles equally - not a search differentiator</t>
+      <c r="LS20" t="inlineStr">
+        <is>
+          <t>Clinic based physician</t>
+        </is>
+      </c>
+      <c r="MB20" t="inlineStr">
+        <is>
+          <t>Community based therapy</t>
+        </is>
+      </c>
+      <c r="MC20" t="inlineStr">
+        <is>
+          <t>Tele rehab 384x216.jpg</t>
+        </is>
+      </c>
+      <c r="ME20" t="inlineStr">
+        <is>
+          <t>Telerehab makes Veterans lives easier</t>
+        </is>
+      </c>
+      <c r="MF20" t="inlineStr">
+        <is>
+          <t>Using Telerehab wheeled mobility clinics. Veterans receive care by bridging the gap for rural access to rehabilitation services. </t>
+        </is>
+      </c>
+      <c r="ML20" t="inlineStr">
+        <is>
+          <t>https://www.vapulse.net/groups/trewi-telerehabilitation-enterprise-wide-initiative</t>
+        </is>
+      </c>
+      <c r="MU20" t="inlineStr">
+        <is>
+          <t>Clarifying implementation of new practice vs new practice in motion</t>
         </is>
       </c>
     </row>
@@ -12233,7 +12633,7 @@
         <v>43705.50811342592</v>
       </c>
       <c r="D24" s="1">
-        <v>43746.34297453704</v>
+        <v>43754.741944444446</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -12257,12 +12657,12 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>On demand tele-geropsychiatry consultation through tele-health. </t>
+          <t>On demand tele-geropsychiatry consultation through telehealth. </t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>Provide rapid consultation on geropsychiatry issues to Veterans across VISN 23. Platforms include tele-health (VA video connect to home, clinical video telehealth) e-consultation and team meetings as requested. </t>
+          <t>Provide rapid consultation on geropsychiatry issues to Veterans across VISN 23. Platforms include telehealth (VA video connect to home, clinical video telehealth) e-consultation and team meetings as requested. </t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
@@ -12297,7 +12697,7 @@
       </c>
       <c r="U24" t="inlineStr">
         <is>
-          <t>VISN23</t>
+          <t>vha_VISN23</t>
         </is>
       </c>
       <c r="V24" t="inlineStr">
@@ -12446,51 +12846,43 @@
           <t>Assoc. Director of tele-mental health </t>
         </is>
       </c>
-      <c r="BT24" t="inlineStr">
+      <c r="BT24">
+        <v>40</v>
+      </c>
+      <c r="BU24">
+        <v>20</v>
+      </c>
+      <c r="BV24" t="inlineStr">
+        <is>
+          <t>5 to 7</t>
+        </is>
+      </c>
+      <c r="BW24">
+        <v>2</v>
+      </c>
+      <c r="BX24">
+        <v>1</v>
+      </c>
+      <c r="BY24" t="inlineStr">
         <is>
           <t>Permanent</t>
         </is>
       </c>
-      <c r="BU24" t="inlineStr">
+      <c r="BZ24" t="inlineStr">
         <is>
           <t>Permanent</t>
         </is>
       </c>
-      <c r="BV24" t="inlineStr">
-        <is>
-          <t>Permanent</t>
-        </is>
-      </c>
-      <c r="BW24" t="inlineStr">
-        <is>
-          <t>Permanent</t>
-        </is>
-      </c>
-      <c r="BX24" t="inlineStr">
-        <is>
-          <t>Permanent</t>
-        </is>
-      </c>
-      <c r="BY24" t="inlineStr">
-        <is>
-          <t>Tele-health equipment. (All tele-health staff on Hub side and pt side).</t>
-        </is>
-      </c>
-      <c r="BZ24" t="inlineStr">
+      <c r="CD24" t="inlineStr">
+        <is>
+          <t>Telehealth equipment. (All tele-health staff on Hub side and pt side).</t>
+        </is>
+      </c>
+      <c r="CE24" t="inlineStr">
         <is>
           <t>Dx, ipads, computers, phone, etc. </t>
         </is>
       </c>
-      <c r="CD24" t="inlineStr">
-        <is>
-          <t>Tele-health equipment. (All tele-health staff on Hub side and pt side).</t>
-        </is>
-      </c>
-      <c r="CE24" t="inlineStr">
-        <is>
-          <t>Dx, ipads, computers, phone, etc. </t>
-        </is>
-      </c>
       <c r="CI24" t="inlineStr">
         <is>
           <t>For Hub employees are trained by Hub. Spoke sites are trained by Spoke FTC</t>
@@ -12528,12 +12920,12 @@
       </c>
       <c r="CY24" t="inlineStr">
         <is>
-          <t>MOU</t>
+          <t>MOU  (Memorandum of Understanding)</t>
         </is>
       </c>
       <c r="CZ24" t="inlineStr">
         <is>
-          <t>TSA</t>
+          <t>TSA  (Telehealth service agreement)</t>
         </is>
       </c>
       <c r="DD24" t="inlineStr">
@@ -12553,12 +12945,22 @@
       </c>
       <c r="DG24" t="inlineStr">
         <is>
-          <t>696x392 placeholder(1).jpg</t>
+          <t>impactHoldrege_696x392.jpg</t>
         </is>
       </c>
       <c r="DH24" t="inlineStr">
         <is>
-          <t>Innovation in Action</t>
+          <t>Innovative Specialty Care in Action-Reaching Veterans in Rural Clinics or in Their Own Homes</t>
+        </is>
+      </c>
+      <c r="DI24" t="inlineStr">
+        <is>
+          <t>Veterans in the rural Heartland are typically several miles from the nearest medical center, be it private or VA. Travel for the older veteran is also complicated by the his/her own physical limitations including inability to drive. By providing geriatric specialty care via telehealth this vulnerable population has timely access to specialty medicine when the need is recognized.</t>
+        </is>
+      </c>
+      <c r="DJ24" t="inlineStr">
+        <is>
+          <t>house696x392.jpg</t>
         </is>
       </c>
       <c r="DP24" t="inlineStr">

</xml_diff>

<commit_message>
DM-DATA: update data import spreadsheet
</commit_message>
<xml_diff>
--- a/lib/assets/Diffusion_Marketplace.xlsx
+++ b/lib/assets/Diffusion_Marketplace.xlsx
@@ -2302,10 +2302,10 @@
         <v>226101601</v>
       </c>
       <c r="C3" s="1">
-        <v>43752.27253472222</v>
+        <v>43752.39753472222</v>
       </c>
       <c r="D3" s="1">
-        <v>43752.29478009259</v>
+        <v>43758.80604166666</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -2551,6 +2551,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="DD3" t="inlineStr">
+        <is>
+          <t>Katie150x150.jpg</t>
+        </is>
+      </c>
       <c r="DE3" t="inlineStr">
         <is>
           <t>How do we put critical resources and coping skills into the hands of those in need?</t>
@@ -2561,6 +2566,11 @@
           <t>Katie Juhasz routinely attended community events to share PTSD resources. Increasingly, people asked for resources for homeless Veterans. Paper handouts weren't particularly durable, and many homeless Veterans do not have reliable access to the internet. Katie wanted something easily accessible and discreet, that would provide useful information in a durable format. The Veterans Crisis Line had plastic-coated wallet cards that people liked; if one card was good, 52 should be great! We created Cards for Connection with the support of an iNet Spark award, and we’re expanding its reach with a Seed award.</t>
         </is>
       </c>
+      <c r="DG3" t="inlineStr">
+        <is>
+          <t>2017 0913 HCD 696x392Workshop.jpg</t>
+        </is>
+      </c>
       <c r="DH3" t="inlineStr">
         <is>
           <t>Our first Human-Centered Design Workshop to flesh out the idea</t>
@@ -2571,6 +2581,11 @@
           <t>During a Human-Centered Design workshop hosted by Drs. Kayt Havens and Shannon McCaslin, we fleshed out the idea for Cards for Connection using content from discovery interviews with two Veterans who work with homeless Veterans, one of whom had previously experienced homelessness. By the end of the workshop we had our first prototype and enough of an idea to start interviews with key stakeholders, to assess acceptability and feasibility for the idea.</t>
         </is>
       </c>
+      <c r="DJ3" t="inlineStr">
+        <is>
+          <t>Cards 696x392.jpg</t>
+        </is>
+      </c>
       <c r="DK3" t="inlineStr">
         <is>
           <t>A Veteran's favorite cards</t>
@@ -2581,6 +2596,11 @@
           <t>We received our first real decks in August 2018. That fall, we conducted focus groups with homeless Veterans living in residential programs to see how they used the cards, and several spontaneously sorted them to identify their favorites. These are the cards selected by one Veteran.</t>
         </is>
       </c>
+      <c r="DM3" t="inlineStr">
+        <is>
+          <t>Thinkofsomething 696x392....jpg</t>
+        </is>
+      </c>
       <c r="DN3" t="inlineStr">
         <is>
           <t>Think of something you're proud of.</t>
@@ -2621,6 +2641,31 @@
           <t>Nicole Muller\Social Worker</t>
         </is>
       </c>
+      <c r="DV3" t="inlineStr">
+        <is>
+          <t>Katie65x65JPG.jpg</t>
+        </is>
+      </c>
+      <c r="DW3" t="inlineStr">
+        <is>
+          <t>Jeremy_65x65.jpg</t>
+        </is>
+      </c>
+      <c r="DX3" t="inlineStr">
+        <is>
+          <t>ElizabethWilliams65x65.jpg</t>
+        </is>
+      </c>
+      <c r="DY3" t="inlineStr">
+        <is>
+          <t>Shannon_65x65.jpg</t>
+        </is>
+      </c>
+      <c r="DZ3" t="inlineStr">
+        <is>
+          <t>Nicole_65x65.jpg</t>
+        </is>
+      </c>
       <c r="EA3" t="inlineStr">
         <is>
           <t>Veteran - Enables an improvement in satisfaction or customer experience for Veterans</t>
@@ -2764,6 +2809,11 @@
       <c r="LV3" t="inlineStr">
         <is>
           <t>Nursing Assistant</t>
+        </is>
+      </c>
+      <c r="MC3" t="inlineStr">
+        <is>
+          <t>384x216AllCards.jpg</t>
         </is>
       </c>
       <c r="MD3" t="inlineStr">
@@ -2795,10 +2845,10 @@
         <v>226101601</v>
       </c>
       <c r="C4" s="1">
-        <v>43749.3374537037</v>
+        <v>43749.4624537037</v>
       </c>
       <c r="D4" s="1">
-        <v>43752.310277777775</v>
+        <v>43758.95018518518</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -2822,7 +2872,7 @@
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>Informing Veterans that they have CKD and how to slow progression through lifestyle change. Veterans enjoy a cooking demonstration, pedometer and resistance band use, along with Medical Nutrition Therapy from a Registered Dietitian. </t>
+          <t>Informing Veterans that they have CKD (Chronic Kideny Disease) and how to slow progression through lifestyle change. Veterans enjoy a cooking demonstration, pedometer and resistance band use, along with Medical Nutrition Therapy from a Registered Dietitian. </t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
@@ -3086,6 +3136,11 @@
           <t>New spread sites receiving funding from iNET will be expected to sign a MOU</t>
         </is>
       </c>
+      <c r="DD4" t="inlineStr">
+        <is>
+          <t>150x150 placeholder copy.jpg</t>
+        </is>
+      </c>
       <c r="DE4" t="inlineStr">
         <is>
           <t>Many who have Chronic Kidney Disease are unaware they have it.</t>
@@ -3354,6 +3409,11 @@
       <c r="LY4" t="inlineStr">
         <is>
           <t>Researcher</t>
+        </is>
+      </c>
+      <c r="MC4" t="inlineStr">
+        <is>
+          <t>384x216 placeholder.jpg</t>
         </is>
       </c>
       <c r="ME4" t="inlineStr">
@@ -3385,10 +3445,10 @@
         <v>241758028</v>
       </c>
       <c r="C5" s="1">
-        <v>43749.31</v>
+        <v>43749.435</v>
       </c>
       <c r="D5" s="1">
-        <v>43749.328206018516</v>
+        <v>43759.023125</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -3427,12 +3487,12 @@
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Mike Moates</t>
+          <t>Dr. Joseph Moates\Provider \Director</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>Sherry Cox</t>
+          <t>Sherry Cox\Rn Facilitator Coach</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
@@ -3442,7 +3502,7 @@
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>Birmingham VA Medical Center</t>
+          <t>vha_521gj</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
@@ -3726,6 +3786,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="DD5" t="inlineStr">
+        <is>
+          <t>150x150 placeholder copy.jpg</t>
+        </is>
+      </c>
       <c r="DE5" t="inlineStr">
         <is>
           <t>Whole Health Opioid Safety Shared Medical Appt.</t>
@@ -3869,6 +3934,11 @@
       <c r="LW5" t="inlineStr">
         <is>
           <t>Pharmacist</t>
+        </is>
+      </c>
+      <c r="MC5" t="inlineStr">
+        <is>
+          <t>384x216 placeholder.jpg</t>
         </is>
       </c>
       <c r="ML5" t="inlineStr">
@@ -3885,10 +3955,10 @@
         <v>241758028</v>
       </c>
       <c r="C6" s="1">
-        <v>43749.26231481481</v>
+        <v>43749.38731481481</v>
       </c>
       <c r="D6" s="1">
-        <v>43749.28013888889</v>
+        <v>43756.05474537037</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -4136,6 +4206,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="DD6" t="inlineStr">
+        <is>
+          <t>150x150 placeholder copy.jpg</t>
+        </is>
+      </c>
       <c r="DE6" t="inlineStr">
         <is>
           <t>Developed by the Robley Rex VA Medical Center for the improvement of the cleanliness and safety of the facility.</t>
@@ -4201,6 +4276,11 @@
           <t>None</t>
         </is>
       </c>
+      <c r="MC6" t="inlineStr">
+        <is>
+          <t>Green Gloves.jpg</t>
+        </is>
+      </c>
       <c r="MD6" t="inlineStr">
         <is>
           <t>https://www.vapulse.va.gov/videos/31083</t>
@@ -4217,6 +4297,11 @@
         </is>
       </c>
       <c r="ML6" t="inlineStr">
+        <is>
+          <t>https://www.vapulse.va.gov/groups/vha-patient-experience/projects/toolkit-green-gloves</t>
+        </is>
+      </c>
+      <c r="MO6" t="inlineStr">
         <is>
           <t>https://www.vapulse.va.gov/groups/vha-patient-experience/projects/toolkit-green-gloves</t>
         </is>
@@ -4230,10 +4315,10 @@
         <v>241758028</v>
       </c>
       <c r="C7" s="1">
-        <v>43747.48888888889</v>
+        <v>43747.61388888889</v>
       </c>
       <c r="D7" s="1">
-        <v>43747.514918981484</v>
+        <v>43758.62125</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -4267,7 +4352,7 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>:  Geriatric Emergency Room Interventions for Veterans (GERI-VET), an evidence-based multidisciplinary program performing geriatric screens and care coordination for at-risk older Veterans treated in the ED, was implemented based on established best practices for Geriatric ED care.  ED staff receive multimodal geriatric emergency medicine training and champion the care of the most frail, older Veterans during their ED visit.  GERI-VET serves as a platform for Geriatric ED Accreditation through the American College of Emergency Physicians.</t>
+          <t>Geriatric Emergency Room Interventions for Veterans (GERI-VET), an evidence-based multidisciplinary program performing geriatric screens and care coordination for at-risk older Veterans treated in the ED, was implemented based on established best practices for Geriatric ED care.  ED staff receive multimodal geriatric emergency medicine training and champion the care of the most frail, older Veterans during their ED visit.  GERI-VET serves as a platform for Geriatric ED Accreditation through the American College of Emergency Physicians.</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
@@ -4469,7 +4554,7 @@
       </c>
       <c r="CI7" t="inlineStr">
         <is>
-          <t>local facility (+/- training through Cleveland GRECC)</t>
+          <t>Local facility (+/- training through Cleveland GRECC)</t>
         </is>
       </c>
       <c r="CJ7" t="inlineStr">
@@ -4497,6 +4582,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="DD7" t="inlineStr">
+        <is>
+          <t>Huded cropped 150x150.jpg</t>
+        </is>
+      </c>
       <c r="DE7" t="inlineStr">
         <is>
           <t>How the VA's first comprehensive geriatric ED program got it's start</t>
@@ -4507,6 +4597,56 @@
           <t>Dr. Huded, Co-Director of GERI-VET, had the opportunity to participate in the multisite GEDI WISE program at Northwestern Memorial Hospital during her Geriatric fellowship.  Wanting to bring a similar evidence-based model of Geriatric ED care to the VHA, she initiated GERI-VET in 2016 with the support of the Cleveland GRECC and VA Innovators Network.  GERI-VET has worked with over a dozen sites in 2018 and 2019 interested in similar programming.</t>
         </is>
       </c>
+      <c r="DG7" t="inlineStr">
+        <is>
+          <t>GV696x392.jpg</t>
+        </is>
+      </c>
+      <c r="DH7" t="inlineStr">
+        <is>
+          <t>Veteran receives Geri-Vet care</t>
+        </is>
+      </c>
+      <c r="DI7" t="inlineStr">
+        <is>
+          <t>Veteran being assessed for physical, psychological, and social factors that impact the older Veterans’ overall health.</t>
+        </is>
+      </c>
+      <c r="DJ7" t="inlineStr">
+        <is>
+          <t>geri  group photo696x392.jpg</t>
+        </is>
+      </c>
+      <c r="DK7" t="inlineStr">
+        <is>
+          <t>Geri-Vet group</t>
+        </is>
+      </c>
+      <c r="DL7" t="inlineStr">
+        <is>
+          <t>Geri- Vet group engages others to works collaboratively to ensure proper measures are in place to treat all Veteran and caregiver needs upon discharge from the ED ( Emergency Department)</t>
+        </is>
+      </c>
+      <c r="DM7" t="inlineStr">
+        <is>
+          <t>GV Bootcamp 696x392.jpg</t>
+        </is>
+      </c>
+      <c r="DN7" t="inlineStr">
+        <is>
+          <t>Geri-vet Boot Camp</t>
+        </is>
+      </c>
+      <c r="DO7" t="inlineStr">
+        <is>
+          <t>GERI-VET program group train to enhance care for Veterans who present to the emergency department.</t>
+        </is>
+      </c>
+      <c r="DP7" t="inlineStr">
+        <is>
+          <t>jill.huded@va.gov</t>
+        </is>
+      </c>
       <c r="DQ7" t="inlineStr">
         <is>
           <t>Dr. Robert Bonomo/Director of Cleveland GRECC</t>
@@ -4522,6 +4662,16 @@
           <t>Dr. Tom Edes/Director of Comprehensive Geriatrics &amp; Palliative Care Clinical Operations</t>
         </is>
       </c>
+      <c r="DU7" t="inlineStr">
+        <is>
+          <t> Jill Huded\Co-Director </t>
+        </is>
+      </c>
+      <c r="DY7" t="inlineStr">
+        <is>
+          <t>Huded cropped 65x65.jpg</t>
+        </is>
+      </c>
       <c r="EA7" t="inlineStr">
         <is>
           <t>Veteran - Enables an improvement in satisfaction or customer experience for Veterans</t>
@@ -4657,6 +4807,11 @@
           <t>Intermediate Care Technician\Licensed Practical Nurse</t>
         </is>
       </c>
+      <c r="MC7" t="inlineStr">
+        <is>
+          <t>GERVET64.384x216.jpg</t>
+        </is>
+      </c>
       <c r="MD7" t="inlineStr">
         <is>
           <t>https://www.youtube.com/watch?v=MDIwu5hQatw</t>
@@ -4672,6 +4827,26 @@
           <t>Dr. Todd Smith discusses the GERI-VET program for the 2018 VA Innovation Experience</t>
         </is>
       </c>
+      <c r="MG7" t="inlineStr">
+        <is>
+          <t>2019 GERI-VET brochure (2).pdf</t>
+        </is>
+      </c>
+      <c r="MH7" t="inlineStr">
+        <is>
+          <t>GERI-VET book for accreditation 10.10.19.pdf</t>
+        </is>
+      </c>
+      <c r="MI7" t="inlineStr">
+        <is>
+          <t>ACEP Cleveland VA Geriatric ED Flyer 5.2019.pdf</t>
+        </is>
+      </c>
+      <c r="MN7" t="inlineStr">
+        <is>
+          <t>FOR IMMEDIATE RELEASE - Cleveland VA Becomes First to Receive Geriatric Emergency Department Accreditation.docx</t>
+        </is>
+      </c>
       <c r="MO7" t="inlineStr">
         <is>
           <t>https://emj.bmj.com/content/35/1/72</t>
@@ -4679,7 +4854,7 @@
       </c>
       <c r="MU7" t="inlineStr">
         <is>
-          <t>wasn't able to upload files :(</t>
+          <t>wasn't able to upload files :(  Impact photo is paid actor. Not real vet. All photos have consent. </t>
         </is>
       </c>
     </row>
@@ -4691,10 +4866,10 @@
         <v>241758028</v>
       </c>
       <c r="C8" s="1">
-        <v>43745.53488425926</v>
+        <v>43745.65988425926</v>
       </c>
       <c r="D8" s="1">
-        <v>43754.33277777778</v>
+        <v>43758.96394675926</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -4761,8 +4936,10 @@
           <t>07/01/2011</t>
         </is>
       </c>
-      <c r="U8">
-        <v>636</v>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>vha_636</t>
+        </is>
       </c>
       <c r="V8" t="inlineStr">
         <is>
@@ -4837,17 +5014,12 @@
       </c>
       <c r="BC8" t="inlineStr">
         <is>
-          <t>dfgsdfg</t>
-        </is>
-      </c>
-      <c r="BE8" t="inlineStr">
-        <is>
-          <t>adsg</t>
-        </is>
-      </c>
-      <c r="BG8" t="inlineStr">
-        <is>
-          <t>sdgsdfg</t>
+          <t>Not using the RAI ( RIsk Assesment Indicator) tool consistantly.</t>
+        </is>
+      </c>
+      <c r="BD8" t="inlineStr">
+        <is>
+          <t>Make it part of new training and create leadership in asking for it everytime. </t>
         </is>
       </c>
       <c r="BI8" t="inlineStr">
@@ -4885,6 +5057,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="DD8" t="inlineStr">
+        <is>
+          <t>150x150 placeholder copy.jpg</t>
+        </is>
+      </c>
       <c r="DP8" t="inlineStr">
         <is>
           <t>Daniel.Hall2@va.gov</t>
@@ -5068,6 +5245,11 @@
       <c r="LW8" t="inlineStr">
         <is>
           <t>Pharmacist</t>
+        </is>
+      </c>
+      <c r="MC8" t="inlineStr">
+        <is>
+          <t>384x216 placeholder.jpg</t>
         </is>
       </c>
     </row>
@@ -5079,10 +5261,10 @@
         <v>241758028</v>
       </c>
       <c r="C9" s="1">
-        <v>43745.47375</v>
+        <v>43745.59875</v>
       </c>
       <c r="D9" s="1">
-        <v>43745.5174537037</v>
+        <v>43758.78134259259</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -5139,8 +5321,10 @@
           <t>01/20/2016</t>
         </is>
       </c>
-      <c r="U9">
-        <v>590</v>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>vha_590</t>
+        </is>
       </c>
       <c r="V9" t="inlineStr">
         <is>
@@ -5413,6 +5597,11 @@
           <t>User Agreement Form</t>
         </is>
       </c>
+      <c r="DD9" t="inlineStr">
+        <is>
+          <t>PRIDE Williams150x150.jpg</t>
+        </is>
+      </c>
       <c r="DE9" t="inlineStr">
         <is>
           <t>Created By Veterans, For Veterans</t>
@@ -5463,6 +5652,11 @@
           <t>Tuscaloosa VA Executive Leadership &amp; Staff</t>
         </is>
       </c>
+      <c r="DX9" t="inlineStr">
+        <is>
+          <t>PRIDE Williams65x65.jpg</t>
+        </is>
+      </c>
       <c r="EA9" t="inlineStr">
         <is>
           <t>Veteran - Enables an improvement in satisfaction or customer experience for Veterans</t>
@@ -5711,6 +5905,11 @@
       <c r="MA9" t="inlineStr">
         <is>
           <t>All job titles equally - not a search differentiator</t>
+        </is>
+      </c>
+      <c r="MC9" t="inlineStr">
+        <is>
+          <t>Pride Placeholder364x216.jpg</t>
         </is>
       </c>
       <c r="MD9" t="inlineStr">
@@ -5747,10 +5946,10 @@
         <v>241758028</v>
       </c>
       <c r="C10" s="1">
-        <v>43742.50230324074</v>
+        <v>43742.62730324074</v>
       </c>
       <c r="D10" s="1">
-        <v>43742.51479166667</v>
+        <v>43756.034317129626</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -5799,7 +5998,7 @@
       </c>
       <c r="U10" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>vha_</t>
         </is>
       </c>
       <c r="V10" t="inlineStr">
@@ -5940,7 +6139,7 @@
       </c>
       <c r="CO10" t="inlineStr">
         <is>
-          <t>Less than 30minutes</t>
+          <t>Less than 30 minutes</t>
         </is>
       </c>
       <c r="CP10" t="inlineStr">
@@ -5958,6 +6157,11 @@
           <t>No</t>
         </is>
       </c>
+      <c r="DD10" t="inlineStr">
+        <is>
+          <t>150x150 placeholder copy.jpg</t>
+        </is>
+      </c>
       <c r="DE10" t="inlineStr">
         <is>
           <t>Addressing the first Moment that Matters most to Veterans in their Outpatient journey.</t>
@@ -6023,7 +6227,17 @@
           <t>All job titles equally - not a search differentiator</t>
         </is>
       </c>
+      <c r="MC10" t="inlineStr">
+        <is>
+          <t>SPG 384x216.jpg</t>
+        </is>
+      </c>
       <c r="ML10" t="inlineStr">
+        <is>
+          <t>https://www.vapulse.va.gov/groups/vha-patient-experience/projects/spg</t>
+        </is>
+      </c>
+      <c r="MO10" t="inlineStr">
         <is>
           <t>https://www.vapulse.va.gov/groups/vha-patient-experience/projects/spg</t>
         </is>
@@ -6037,10 +6251,10 @@
         <v>241758028</v>
       </c>
       <c r="C11" s="1">
-        <v>43742.421423611115</v>
+        <v>43742.546423611115</v>
       </c>
       <c r="D11" s="1">
-        <v>43742.45453703704</v>
+        <v>43756.024247685185</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -6399,7 +6613,32 @@
           <t>None</t>
         </is>
       </c>
+      <c r="MC11" t="inlineStr">
+        <is>
+          <t>- PatientAmbassador384x216 pdf.jpg</t>
+        </is>
+      </c>
+      <c r="MD11" t="inlineStr">
+        <is>
+          <t>https://youtu.be/tH-EEV8z1rs</t>
+        </is>
+      </c>
+      <c r="ME11" t="inlineStr">
+        <is>
+          <t>Improving the Veteran Experience: Red Coat Ambassadors</t>
+        </is>
+      </c>
+      <c r="MF11" t="inlineStr">
+        <is>
+          <t>How RCA makes it easie for Veterans </t>
+        </is>
+      </c>
       <c r="ML11" t="inlineStr">
+        <is>
+          <t>https://www.vapulse.va.gov/groups/vha-patient-experience/projects/toolkit-red-coat-ambassadors</t>
+        </is>
+      </c>
+      <c r="MO11" t="inlineStr">
         <is>
           <t>https://www.vapulse.va.gov/groups/vha-patient-experience/projects/toolkit-red-coat-ambassadors</t>
         </is>
@@ -6413,10 +6652,10 @@
         <v>241758028</v>
       </c>
       <c r="C12" s="1">
-        <v>43742.23888888889</v>
+        <v>43742.36388888889</v>
       </c>
       <c r="D12" s="1">
-        <v>43746.624074074076</v>
+        <v>43758.816400462965</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -6483,8 +6722,10 @@
           <t>09/01/2018</t>
         </is>
       </c>
-      <c r="U12">
-        <v>652</v>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>vha_652</t>
+        </is>
       </c>
       <c r="V12" t="inlineStr">
         <is>
@@ -6562,146 +6803,126 @@
           <t>We plan to only use the secure, HIPAA-compliant CPRS system to collect patient outcome information. </t>
         </is>
       </c>
-      <c r="BE12" t="inlineStr">
+      <c r="BI12" t="inlineStr">
+        <is>
+          <t>3. $50,000 - $250,000</t>
+        </is>
+      </c>
+      <c r="BJ12" t="inlineStr">
+        <is>
+          <t>2. Some complexity</t>
+        </is>
+      </c>
+      <c r="BK12" t="inlineStr">
+        <is>
+          <t>1. Little to no complexity</t>
+        </is>
+      </c>
+      <c r="BL12" t="inlineStr">
+        <is>
+          <t>1. Single department</t>
+        </is>
+      </c>
+      <c r="BM12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="BN12" t="inlineStr">
+        <is>
+          <t>New Clinical Approach or New Process</t>
+        </is>
+      </c>
+      <c r="BO12" t="inlineStr">
+        <is>
+          <t>Social Worker</t>
+        </is>
+      </c>
+      <c r="BP12" t="inlineStr">
+        <is>
+          <t>Psychologist</t>
+        </is>
+      </c>
+      <c r="BT12" t="inlineStr">
+        <is>
+          <t>No more hours than what is already expected as part of standard care</t>
+        </is>
+      </c>
+      <c r="BU12" t="inlineStr">
+        <is>
+          <t>No more hours than what is already expected as part of standard care</t>
+        </is>
+      </c>
+      <c r="BY12" t="inlineStr">
+        <is>
+          <t>The same as would typically be required for treatment, they will just be using their time more efficiently </t>
+        </is>
+      </c>
+      <c r="BZ12" t="inlineStr">
+        <is>
+          <t>The same as would typically be required for treatment, they will just be using their time more efficiently </t>
+        </is>
+      </c>
+      <c r="CD12" t="inlineStr">
+        <is>
+          <t>TST Individual Client Book (free of charge)</t>
+        </is>
+      </c>
+      <c r="CE12" t="inlineStr">
+        <is>
+          <t>TST Individual Facilitator Book (free of charge)</t>
+        </is>
+      </c>
+      <c r="CF12" t="inlineStr">
+        <is>
+          <t>TST Group Client Book (free of charge)</t>
+        </is>
+      </c>
+      <c r="CG12" t="inlineStr">
+        <is>
+          <t>TST Group Facilitator Book (free of charge)</t>
+        </is>
+      </c>
+      <c r="CI12" t="inlineStr">
+        <is>
+          <t>TST developers host train-the-trainers workshops. Attendees of this one-to-two-day workshop then become TST trainers.</t>
+        </is>
+      </c>
+      <c r="CJ12" t="inlineStr">
+        <is>
+          <t>Anyone who is planning to use TST with their clients must receive training (such as social workers and psychologists)</t>
+        </is>
+      </c>
+      <c r="CO12" t="inlineStr">
+        <is>
+          <t>One to two days long</t>
+        </is>
+      </c>
+      <c r="CP12" t="inlineStr">
+        <is>
+          <t>Providers who would like to be TST trainers must attend a two-day train-the-trainers workshop. Providers who would like to be trained in TST must attend a one to two-day training workshop hosted by a TST trainer.  </t>
+        </is>
+      </c>
+      <c r="CQ12" t="inlineStr">
+        <is>
+          <t>Potentially</t>
+        </is>
+      </c>
+      <c r="CR12" t="inlineStr">
+        <is>
+          <t>Can be free to charge </t>
+        </is>
+      </c>
+      <c r="CX12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="CY12" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="BF12" t="inlineStr">
-        <is>
-          <t>N/A </t>
-        </is>
-      </c>
-      <c r="BG12" t="inlineStr">
-        <is>
-          <t>N/A </t>
-        </is>
-      </c>
-      <c r="BH12" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="BI12" t="inlineStr">
-        <is>
-          <t>3. $50,000 - $250,000</t>
-        </is>
-      </c>
-      <c r="BJ12" t="inlineStr">
-        <is>
-          <t>2. Some complexity</t>
-        </is>
-      </c>
-      <c r="BK12" t="inlineStr">
-        <is>
-          <t>1. Little to no complexity</t>
-        </is>
-      </c>
-      <c r="BL12" t="inlineStr">
-        <is>
-          <t>1. Single department</t>
-        </is>
-      </c>
-      <c r="BM12" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="BN12" t="inlineStr">
-        <is>
-          <t>New Clinical Approach or New Process</t>
-        </is>
-      </c>
-      <c r="BO12" t="inlineStr">
-        <is>
-          <t>Social Worker</t>
-        </is>
-      </c>
-      <c r="BP12" t="inlineStr">
-        <is>
-          <t>Psychologist</t>
-        </is>
-      </c>
-      <c r="BT12" t="inlineStr">
-        <is>
-          <t>No more hours than what is already expected as part of standard care</t>
-        </is>
-      </c>
-      <c r="BU12" t="inlineStr">
-        <is>
-          <t>No more hours than what is already expected as part of standard care</t>
-        </is>
-      </c>
-      <c r="BY12" t="inlineStr">
-        <is>
-          <t>The same as would typically be required for treatment, they will just be using their time more efficiently </t>
-        </is>
-      </c>
-      <c r="BZ12" t="inlineStr">
-        <is>
-          <t>The same as would typically be required for treatment, they will just be using their time more efficiently </t>
-        </is>
-      </c>
-      <c r="CD12" t="inlineStr">
-        <is>
-          <t>TST Individual Client Book (free of charge)</t>
-        </is>
-      </c>
-      <c r="CE12" t="inlineStr">
-        <is>
-          <t>TST Individual Facilitator Book (free of charge)</t>
-        </is>
-      </c>
-      <c r="CF12" t="inlineStr">
-        <is>
-          <t>TST Group Client Book (free of charge)</t>
-        </is>
-      </c>
-      <c r="CG12" t="inlineStr">
-        <is>
-          <t>TST Group Facilitator Book (free of charge)</t>
-        </is>
-      </c>
-      <c r="CI12" t="inlineStr">
-        <is>
-          <t>TST developers host train-the-trainers workshops. Attendees of this one-to-two-day workshop then become TST trainers.</t>
-        </is>
-      </c>
-      <c r="CJ12" t="inlineStr">
-        <is>
-          <t>Anyone who is planning to use TST with their clients must receive training (such as social workers and psychologists)</t>
-        </is>
-      </c>
-      <c r="CO12" t="inlineStr">
-        <is>
-          <t>One to two days long</t>
-        </is>
-      </c>
-      <c r="CP12" t="inlineStr">
-        <is>
-          <t>Providers who would like to be TST trainers must attend a two-day train-the-trainers workshop. Providers who would like to be trained in TST must attend a one to two-day training workshop hosted by a TST trainer.  </t>
-        </is>
-      </c>
-      <c r="CQ12" t="inlineStr">
-        <is>
-          <t>Potentially</t>
-        </is>
-      </c>
-      <c r="CR12" t="inlineStr">
-        <is>
-          <t>Can be free to charge </t>
-        </is>
-      </c>
-      <c r="CX12" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="CY12" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
       <c r="DD12" t="inlineStr">
         <is>
           <t>2019 Head Shot.jpg</t>
@@ -6867,9 +7088,14 @@
           <t>Psychologist\Social Worker</t>
         </is>
       </c>
-      <c r="ME12" t="inlineStr">
-        <is>
-          <t>Video to be added later</t>
+      <c r="MC12" t="inlineStr">
+        <is>
+          <t>384x216 placeholder.jpg</t>
+        </is>
+      </c>
+      <c r="MG12" t="inlineStr">
+        <is>
+          <t>TST Journal 4-24-19(1).pdf</t>
         </is>
       </c>
       <c r="MJ12" t="inlineStr">
@@ -6896,10 +7122,10 @@
         <v>241758028</v>
       </c>
       <c r="C13" s="1">
-        <v>43738.31664351852</v>
+        <v>43738.44164351852</v>
       </c>
       <c r="D13" s="1">
-        <v>43738.34155092593</v>
+        <v>43755.81554398148</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -6943,12 +7169,12 @@
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Michael Broady</t>
+          <t>Michael Broady\CSM(R), MHRM  Patient Experience (PX) Consultant/Facilitator</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Cajun Comeau</t>
+          <t>Cajun Comeau\Patient Experience Consultant</t>
         </is>
       </c>
       <c r="T13" t="inlineStr">
@@ -7034,7 +7260,12 @@
       </c>
       <c r="BC13" t="inlineStr">
         <is>
-          <t>jsbdjbsdjf</t>
+          <t>Team does not adopt and work together, lack of patient engagement</t>
+        </is>
+      </c>
+      <c r="BD13" t="inlineStr">
+        <is>
+          <t>Connection and leading by example through multiple disiplines through a team coach. </t>
         </is>
       </c>
       <c r="BI13" t="inlineStr">
@@ -7069,7 +7300,7 @@
       </c>
       <c r="CD13" t="inlineStr">
         <is>
-          <t>Training</t>
+          <t>Training/Trainer</t>
         </is>
       </c>
       <c r="CE13" t="inlineStr">
@@ -7084,7 +7315,7 @@
       </c>
       <c r="CJ13" t="inlineStr">
         <is>
-          <t>VA support and clinicain staff </t>
+          <t>VA support and clinic staff </t>
         </is>
       </c>
       <c r="CO13" t="inlineStr">
@@ -7112,11 +7343,81 @@
           <t>No</t>
         </is>
       </c>
+      <c r="DD13" t="inlineStr">
+        <is>
+          <t>150x150TOD.jpg</t>
+        </is>
+      </c>
+      <c r="DE13" t="inlineStr">
+        <is>
+          <t>Military Cultural Competency - Veterans and Employee Experience orientation </t>
+        </is>
+      </c>
+      <c r="DF13" t="inlineStr">
+        <is>
+          <t>Understanding and using Military Cultural Competency (MCC) to connect more viscerally with Veterans at the VA is a “not a nice to have”, it is a required skill set in the NEW  Veterans and Employee Experience oriented VA.  If we are to enhance the Veteran and Employee experience, we must provide the training necessary to make our VA workforce feel more confident and valued…presently, very few get any training and learn on the job often dealing with difficult Veterans relying on a limited skill set. Our VA professionals and Veterans deserve better!   MCC is also about healing relationships based on interactions and conversations that change the way Veterans feel about their value, employees, and their over-all VA experience.    </t>
+        </is>
+      </c>
+      <c r="DG13" t="inlineStr">
+        <is>
+          <t>ToD Impact696x392(1).jpg</t>
+        </is>
+      </c>
+      <c r="DH13" t="inlineStr">
+        <is>
+          <t>What matters to Veterans matters to us!</t>
+        </is>
+      </c>
+      <c r="DI13" t="inlineStr">
+        <is>
+          <t>Understanding military culture, creating environments for caring. Whole health ideals for veterans and their support community.   </t>
+        </is>
+      </c>
+      <c r="DJ13" t="inlineStr">
+        <is>
+          <t>So help me impact-696x392png.jpg</t>
+        </is>
+      </c>
+      <c r="DK13" t="inlineStr">
+        <is>
+          <t>Shared Ethos</t>
+        </is>
+      </c>
+      <c r="DL13" t="inlineStr">
+        <is>
+          <t>If you are a Veteran, I am sure that you immediately recognize the words shown here as an oath that you took when you joined the military.  Civil Servants take the same oath… think about what that oath actually says….it ties in nicely with our ICARE values/ethos.  The commitment we take to raise our hand and take a Federal Oath is not to be taken lightly!  It is a promise and commitment that compels you to do the right thing and protect and defend the constitution of the United States.  The oath doesn’t discuss caring for Veterans, but that is certainly implied.  It directly speaks to the larger calling of serving our nation, without a uniform; Civil and Public Service.  The Military takes a variation of the same exact Federal oath.  Our nation could not function with just a military; there must always be others willing to care for and save lives in the Homeland…at the VA.  The oath is much more than ceremonial, it is dedication the highest ideals and commitment to our nation!    It is not enough to take the oath without truly understanding what it stands for.  In large Government organizations over time, a re-commitment and study of the importance of the oath is required to keep the force inspired, valued and motivated.    </t>
+        </is>
+      </c>
+      <c r="DM13" t="inlineStr">
+        <is>
+          <t>ToD3 696x392.jpg</t>
+        </is>
+      </c>
+      <c r="DN13" t="inlineStr">
+        <is>
+          <t>Valued</t>
+        </is>
+      </c>
+      <c r="DO13" t="inlineStr">
+        <is>
+          <t>The Practice of Whole Health for the VA workforce combines exploring what matters most to an individual along with empowering them to action with self care strategies to support their bodies own self healing capabilities while providing excellent clinical care through our professional care while also connecting them to helpful resources within their community. Employee-centered practice affirms the importance of the relationship + partnership between you and fellow employees. This includes focus on self-care and the entire VA workforce community.  If leaders say “I really care about my workforce” whole health as a workforce strategy can make those words actionable…people can feel that they are valued  </t>
+        </is>
+      </c>
+      <c r="DP13" t="inlineStr">
+        <is>
+          <t>Michael.Broady@va.gov</t>
+        </is>
+      </c>
       <c r="DQ13" t="inlineStr">
         <is>
           <t>Michael Broady/CSM(R), MHRM  Patient Experience (PX) Consultant/Facilitator</t>
         </is>
       </c>
+      <c r="DR13" t="inlineStr">
+        <is>
+          <t>Cajun Comeau\Patient Experience Consultant</t>
+        </is>
+      </c>
       <c r="EA13" t="inlineStr">
         <is>
           <t>Veteran - Enables an improvement in satisfaction or customer experience for Veterans</t>
@@ -7195,6 +7496,11 @@
       <c r="MA13" t="inlineStr">
         <is>
           <t>All job titles equally - not a search differentiator</t>
+        </is>
+      </c>
+      <c r="MC13" t="inlineStr">
+        <is>
+          <t>ToD384x216.jpg</t>
         </is>
       </c>
       <c r="ML13" t="inlineStr">
@@ -7211,10 +7517,10 @@
         <v>241758028</v>
       </c>
       <c r="C14" s="1">
-        <v>43734.89344907407</v>
+        <v>43735.01844907407</v>
       </c>
       <c r="D14" s="1">
-        <v>43738.30342592593</v>
+        <v>43759.0365625</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -7278,7 +7584,7 @@
       </c>
       <c r="U14" t="inlineStr">
         <is>
-          <t>VA_588</t>
+          <t>vha_588</t>
         </is>
       </c>
       <c r="V14" t="inlineStr">
@@ -7918,10 +8224,10 @@
         <v>241758028</v>
       </c>
       <c r="C15" s="1">
-        <v>43734.60157407408</v>
+        <v>43734.72657407408</v>
       </c>
       <c r="D15" s="1">
-        <v>43754.683333333334</v>
+        <v>43754.808333333334</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -8436,10 +8742,10 @@
         <v>241758028</v>
       </c>
       <c r="C16" s="1">
-        <v>43728.38668981481</v>
+        <v>43728.51168981481</v>
       </c>
       <c r="D16" s="1">
-        <v>43731.31579861111</v>
+        <v>43759.03747685185</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -8488,7 +8794,7 @@
       </c>
       <c r="U16" t="inlineStr">
         <is>
-          <t>636A6</t>
+          <t>vha_636A6</t>
         </is>
       </c>
       <c r="V16" t="inlineStr">
@@ -9016,10 +9322,10 @@
         <v>241758028</v>
       </c>
       <c r="C17" s="1">
-        <v>43728.34165509259</v>
+        <v>43728.46665509259</v>
       </c>
       <c r="D17" s="1">
-        <v>43749.24946759259</v>
+        <v>43749.37446759259</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -9356,10 +9662,10 @@
         <v>241758028</v>
       </c>
       <c r="C18" s="1">
-        <v>43727.2680787037</v>
+        <v>43727.3930787037</v>
       </c>
       <c r="D18" s="1">
-        <v>43741.46246527778</v>
+        <v>43758.843668981484</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -9426,8 +9732,10 @@
           <t>08/24/2018</t>
         </is>
       </c>
-      <c r="U18">
-        <v>600</v>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>vha_600</t>
+        </is>
       </c>
       <c r="V18" t="inlineStr">
         <is>
@@ -9502,7 +9810,7 @@
       </c>
       <c r="AL18" t="inlineStr">
         <is>
-          <t>two weeks</t>
+          <t>Two weeks</t>
         </is>
       </c>
       <c r="AM18" t="inlineStr">
@@ -9512,7 +9820,7 @@
       </c>
       <c r="AN18" t="inlineStr">
         <is>
-          <t>ongoing </t>
+          <t>Ongoing </t>
         </is>
       </c>
       <c r="AS18" t="inlineStr">
@@ -9527,12 +9835,12 @@
       </c>
       <c r="BD18" t="inlineStr">
         <is>
-          <t>ongoing continued rick assesment and training</t>
+          <t>Ongoing continued rick assesment and training</t>
         </is>
       </c>
       <c r="BE18" t="inlineStr">
         <is>
-          <t>inneffective or undertrained staff </t>
+          <t>Inneffective or undertrained staff </t>
         </is>
       </c>
       <c r="BF18" t="inlineStr">
@@ -9542,7 +9850,7 @@
       </c>
       <c r="BG18" t="inlineStr">
         <is>
-          <t>lack of support and collaboration</t>
+          <t>Lack of support and collaboration</t>
         </is>
       </c>
       <c r="BH18" t="inlineStr">
@@ -9692,6 +10000,11 @@
           <t>902 request</t>
         </is>
       </c>
+      <c r="DD18" t="inlineStr">
+        <is>
+          <t>vmet 150x150.jpg</t>
+        </is>
+      </c>
       <c r="DE18" t="inlineStr">
         <is>
           <t>Mitigating incareration, Deesculating crisis, and expiditing access to care</t>
@@ -9702,6 +10015,11 @@
           <t>VMET is a proactive utilization of VA Police officers in conjunction with Mental Health Clinicians to conduct outreach and follow-up on cases of veterans experiencing mental health crises, additionally those veterans expressing a danger to self, others, and inability to care for themselves.   By pairing a social worker with police, the engagement process could potentially decrease the veteran’s anxiety and barriers, providing an opportunity for veterans to receive the appropriate treatment unique to their needs.  VMET reduces veterans from ending up in jail or at a local hospital where continuity of care is extremely difficult. First program of its kind.</t>
         </is>
       </c>
+      <c r="DG18" t="inlineStr">
+        <is>
+          <t>jumper692x392.jpg</t>
+        </is>
+      </c>
       <c r="DH18" t="inlineStr">
         <is>
           <t>The Jumper</t>
@@ -9712,6 +10030,11 @@
           <t>This is an image of a suicidal veteran on a call we went on who was wanted to jump after being frustrated about his VA benefits. Through VMET, we were able to deescalate and bring the veteran to safety. He was brought back to VA for VA care. </t>
         </is>
       </c>
+      <c r="DJ18" t="inlineStr">
+        <is>
+          <t>HOUSE692x392.jpg</t>
+        </is>
+      </c>
       <c r="DK18" t="inlineStr">
         <is>
           <t>House to Home</t>
@@ -9722,6 +10045,11 @@
           <t>This is a call for service to a veteran who was Gravely disabled. With joint effort of local law enforcement, we were able to place the veteran on a psychiatric care and prevent danger to the veteran, his family and community providers.  He was ultimately bought to VA for mental health treatment and substance abuse and housing services. </t>
         </is>
       </c>
+      <c r="DM18" t="inlineStr">
+        <is>
+          <t>in action696x392.jpg</t>
+        </is>
+      </c>
       <c r="DN18" t="inlineStr">
         <is>
           <t>In Action- Crisis Call</t>
@@ -9762,6 +10090,31 @@
           <t>Walt Dannenberg/ Director Tibor RUbin VA </t>
         </is>
       </c>
+      <c r="DV18" t="inlineStr">
+        <is>
+          <t>shannon head shot65x65.jpg</t>
+        </is>
+      </c>
+      <c r="DW18" t="inlineStr">
+        <is>
+          <t>tbone headshot65x65.jpg</t>
+        </is>
+      </c>
+      <c r="DX18" t="inlineStr">
+        <is>
+          <t>hayter65x65.jpg</t>
+        </is>
+      </c>
+      <c r="DY18" t="inlineStr">
+        <is>
+          <t>Carol65x65.png</t>
+        </is>
+      </c>
+      <c r="DZ18" t="inlineStr">
+        <is>
+          <t>Dannenberg Official Portrait (65x65)(1).jpg</t>
+        </is>
+      </c>
       <c r="EA18" t="inlineStr">
         <is>
           <t>Veteran - Enables an improvement in satisfaction or customer experience for Veterans</t>
@@ -9897,6 +10250,11 @@
           <t>Social Work/Police</t>
         </is>
       </c>
+      <c r="MC18" t="inlineStr">
+        <is>
+          <t>JP intervention384x216.jpg</t>
+        </is>
+      </c>
       <c r="MD18" t="inlineStr">
         <is>
           <t>https://www.wunc.org/post/help-veterans-crisis-va-counselors-are-riding-along-police</t>
@@ -9910,6 +10268,21 @@
       <c r="MF18" t="inlineStr">
         <is>
           <t>This is an interview done about VMET and story published </t>
+        </is>
+      </c>
+      <c r="ML18" t="inlineStr">
+        <is>
+          <t> https://www.vapulse.net/docs/DOC-265342</t>
+        </is>
+      </c>
+      <c r="MO18" t="inlineStr">
+        <is>
+          <t> https://www.washingtonpost.com/national/veterans-talking-veterans-back-from-the-brink-a-new-approach-to-policing-and-lives-in-crisis/2019/03/20/c1add29e-4508-11e9-8aab-95b8d80a1e4f_story.html</t>
+        </is>
+      </c>
+      <c r="MP18" t="inlineStr">
+        <is>
+          <t>https://www.blogs.va.gov/VAntage/60186/va-and-law-enforcement-partnership-supports-veterans-in-need/</t>
         </is>
       </c>
       <c r="MT18" t="inlineStr">
@@ -9931,10 +10304,10 @@
         <v>241758028</v>
       </c>
       <c r="C19" s="1">
-        <v>43713.30734953703</v>
+        <v>43713.43234953703</v>
       </c>
       <c r="D19" s="1">
-        <v>43746.31810185185</v>
+        <v>43746.44310185185</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -10406,10 +10779,10 @@
         <v>241758028</v>
       </c>
       <c r="C20" s="1">
-        <v>43713.234456018516</v>
+        <v>43713.359456018516</v>
       </c>
       <c r="D20" s="1">
-        <v>43755.35863425926</v>
+        <v>43755.48363425926</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -11151,10 +11524,10 @@
         <v>241758028</v>
       </c>
       <c r="C21" s="1">
-        <v>43711.37951388889</v>
+        <v>43711.50451388889</v>
       </c>
       <c r="D21" s="1">
-        <v>43746.379791666666</v>
+        <v>43746.504791666666</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -11621,10 +11994,10 @@
         <v>241758028</v>
       </c>
       <c r="C22" s="1">
-        <v>43707.321122685185</v>
+        <v>43707.446122685185</v>
       </c>
       <c r="D22" s="1">
-        <v>43746.37315972222</v>
+        <v>43746.49815972222</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -12029,10 +12402,10 @@
         <v>241758028</v>
       </c>
       <c r="C23" s="1">
-        <v>43705.685625</v>
+        <v>43705.810625</v>
       </c>
       <c r="D23" s="1">
-        <v>43744.95313657408</v>
+        <v>43745.07813657408</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -12630,10 +13003,10 @@
         <v>241758028</v>
       </c>
       <c r="C24" s="1">
-        <v>43705.50811342592</v>
+        <v>43705.63311342592</v>
       </c>
       <c r="D24" s="1">
-        <v>43754.741944444446</v>
+        <v>43759.01363425926</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -12697,7 +13070,7 @@
       </c>
       <c r="U24" t="inlineStr">
         <is>
-          <t>vha_VISN23</t>
+          <t>vha_23</t>
         </is>
       </c>
       <c r="V24" t="inlineStr">
@@ -12783,7 +13156,7 @@
       </c>
       <c r="BG24" t="inlineStr">
         <is>
-          <t>Sensory and cognitive deficit of pt population. </t>
+          <t>Sensory and cognitive deficit of patient population. </t>
         </is>
       </c>
       <c r="BH24" t="inlineStr">
@@ -13407,10 +13780,10 @@
         <v>241758028</v>
       </c>
       <c r="C25" s="1">
-        <v>43689.29115740741</v>
+        <v>43689.41615740741</v>
       </c>
       <c r="D25" s="1">
-        <v>43693.56576388889</v>
+        <v>43693.69076388889</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -13935,10 +14308,10 @@
         <v>241758028</v>
       </c>
       <c r="C26" s="1">
-        <v>43687.47125</v>
+        <v>43687.59625</v>
       </c>
       <c r="D26" s="1">
-        <v>43745.7534375</v>
+        <v>43745.8784375</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -14560,10 +14933,10 @@
         <v>241758028</v>
       </c>
       <c r="C27" s="1">
-        <v>43685.49167824074</v>
+        <v>43685.61667824074</v>
       </c>
       <c r="D27" s="1">
-        <v>43745.78134259259</v>
+        <v>43759.03574074074</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -14630,8 +15003,10 @@
           <t>08/01/0014</t>
         </is>
       </c>
-      <c r="U27">
-        <v>542</v>
+      <c r="U27" t="inlineStr">
+        <is>
+          <t>vha_542</t>
+        </is>
       </c>
       <c r="V27" t="inlineStr">
         <is>
@@ -15248,10 +15623,10 @@
         <v>241758028</v>
       </c>
       <c r="C28" s="1">
-        <v>43685.440405092595</v>
+        <v>43685.565405092595</v>
       </c>
       <c r="D28" s="1">
-        <v>43709.903495370374</v>
+        <v>43759.0384375</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -15318,8 +15693,10 @@
           <t>09/01/2014</t>
         </is>
       </c>
-      <c r="U28">
-        <v>607</v>
+      <c r="U28" t="inlineStr">
+        <is>
+          <t>vha_607</t>
+        </is>
       </c>
       <c r="V28" t="inlineStr">
         <is>
@@ -15971,10 +16348,10 @@
         <v>241758028</v>
       </c>
       <c r="C29" s="1">
-        <v>43677.60171296296</v>
+        <v>43677.72671296296</v>
       </c>
       <c r="D29" s="1">
-        <v>43744.340104166666</v>
+        <v>43758.76136574074</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -16008,7 +16385,7 @@
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>Home Sleep Apnea Testing is sharply increasing to meet Veteran demands.  Implementation of a home sleep apnea testing program has become an intragal part of the Sleep Medicine Program Office as a way to address access issues.  Implementation of a home sleep testing program bring many beneifts to sleep programs such as reduced costs over Community Care and Veteran travel.  It also opens opportunities to partner with another VA through inter and intrafacility agreements for scoring and interpretation.</t>
+          <t>Utilization of home sleep apnea testing (HSAT) to diagnose sleep apnea is rapidly increasing to better meet demand for Veteran evaluation of suspected OSA (Obstructive Sleep Apnea). HSAT( Home Sleep Apnea Testing) is considered a best practice and is supported by the Office of Specialty Care Services, Telehealth Service, and Office of Veteran Access to Care. Home Sleep Apnea Testing is sharply increasing to meet Veteran demands.  Implementation of a home sleep apnea testing program has become an intragal part of the Sleep Medicine Program Office as a way to address access issues.  Implementation of a home sleep testing program bring many beneifts to sleep programs such as reduced costs over Community Care and Veteran travel.  It also opens opportunities to partner with another VA through inter and intrafacility agreements for scoring and interpretation.</t>
         </is>
       </c>
       <c r="O29" t="inlineStr">
@@ -16405,6 +16782,11 @@
       <c r="MB29" t="inlineStr">
         <is>
           <t>Respiratory Therapist\ Sleep Tech\Telehealth Technician</t>
+        </is>
+      </c>
+      <c r="MC29" t="inlineStr">
+        <is>
+          <t>TeleHealth Sleep Apnea Placeholder384x216.jpg</t>
         </is>
       </c>
       <c r="ML29" t="inlineStr">
@@ -16426,10 +16808,10 @@
         <v>241758028</v>
       </c>
       <c r="C30" s="1">
-        <v>43676.40510416667</v>
+        <v>43676.53010416667</v>
       </c>
       <c r="D30" s="1">
-        <v>43744.894375</v>
+        <v>43745.019375</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -16836,10 +17218,10 @@
         <v>226101601</v>
       </c>
       <c r="C31" s="1">
-        <v>43621.13875</v>
+        <v>43621.26375</v>
       </c>
       <c r="D31" s="1">
-        <v>43661.91153935185</v>
+        <v>43759.041967592595</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -16903,7 +17285,7 @@
       </c>
       <c r="U31" t="inlineStr">
         <is>
-          <t>Long Beach VA Health Care System</t>
+          <t>vha_600</t>
         </is>
       </c>
       <c r="V31" t="inlineStr">
@@ -17294,10 +17676,10 @@
         <v>226101601</v>
       </c>
       <c r="C32" s="1">
-        <v>43620.515173611115</v>
+        <v>43620.640173611115</v>
       </c>
       <c r="D32" s="1">
-        <v>43642.424791666665</v>
+        <v>43642.549791666665</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -17668,10 +18050,10 @@
         <v>226101601</v>
       </c>
       <c r="C33" s="1">
-        <v>43613.30701388889</v>
+        <v>43613.43201388889</v>
       </c>
       <c r="D33" s="1">
-        <v>43620.64811342592</v>
+        <v>43620.77311342592</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -18145,10 +18527,10 @@
         <v>226101601</v>
       </c>
       <c r="C34" s="1">
-        <v>43609.363969907405</v>
+        <v>43609.488969907405</v>
       </c>
       <c r="D34" s="1">
-        <v>43619.38792824074</v>
+        <v>43619.51292824074</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -18501,10 +18883,10 @@
         <v>233326486</v>
       </c>
       <c r="C35" s="1">
-        <v>43607.5493287037</v>
+        <v>43607.6743287037</v>
       </c>
       <c r="D35" s="1">
-        <v>43627.494791666664</v>
+        <v>43627.619791666664</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -19132,10 +19514,10 @@
         <v>226101601</v>
       </c>
       <c r="C36" s="1">
-        <v>43605.433842592596</v>
+        <v>43605.558842592596</v>
       </c>
       <c r="D36" s="1">
-        <v>43728.30571759259</v>
+        <v>43728.43071759259</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -19496,10 +19878,10 @@
         <v>233326486</v>
       </c>
       <c r="C37" s="1">
-        <v>43603.492210648146</v>
+        <v>43603.617210648146</v>
       </c>
       <c r="D37" s="1">
-        <v>43671.48233796296</v>
+        <v>43671.60733796296</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -20066,10 +20448,10 @@
         <v>233326486</v>
       </c>
       <c r="C38" s="1">
-        <v>43602.46909722222</v>
+        <v>43602.59409722222</v>
       </c>
       <c r="D38" s="1">
-        <v>43671.491435185184</v>
+        <v>43671.616435185184</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -20726,10 +21108,10 @@
         <v>226101601</v>
       </c>
       <c r="C39" s="1">
-        <v>43602.236655092594</v>
+        <v>43602.361655092594</v>
       </c>
       <c r="D39" s="1">
-        <v>43628.58248842593</v>
+        <v>43628.70748842593</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -21276,10 +21658,10 @@
         <v>226101601</v>
       </c>
       <c r="C40" s="1">
-        <v>43602.20869212963</v>
+        <v>43602.33369212963</v>
       </c>
       <c r="D40" s="1">
-        <v>43622.58247685185</v>
+        <v>43622.70747685185</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -21616,10 +21998,10 @@
         <v>233326486</v>
       </c>
       <c r="C41" s="1">
-        <v>43601.2716087963</v>
+        <v>43601.3966087963</v>
       </c>
       <c r="D41" s="1">
-        <v>43627.49894675926</v>
+        <v>43627.62394675926</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -22054,10 +22436,10 @@
         <v>226101601</v>
       </c>
       <c r="C42" s="1">
-        <v>43601.179976851854</v>
+        <v>43601.304976851854</v>
       </c>
       <c r="D42" s="1">
-        <v>43619.450208333335</v>
+        <v>43619.575208333335</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -22740,10 +23122,10 @@
         <v>233326486</v>
       </c>
       <c r="C43" s="1">
-        <v>43600.57394675926</v>
+        <v>43600.69894675926</v>
       </c>
       <c r="D43" s="1">
-        <v>43622.558020833334</v>
+        <v>43622.683020833334</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -23185,10 +23567,10 @@
         <v>233326486</v>
       </c>
       <c r="C44" s="1">
-        <v>43600.448275462964</v>
+        <v>43600.573275462964</v>
       </c>
       <c r="D44" s="1">
-        <v>43619.446064814816</v>
+        <v>43619.571064814816</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -23503,10 +23885,10 @@
         <v>226101601</v>
       </c>
       <c r="C45" s="1">
-        <v>43599.483715277776</v>
+        <v>43599.608715277776</v>
       </c>
       <c r="D45" s="1">
-        <v>43616.412824074076</v>
+        <v>43616.537824074076</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -24088,10 +24470,10 @@
         <v>233318351</v>
       </c>
       <c r="C46" s="1">
-        <v>43594.368946759256</v>
+        <v>43594.493946759256</v>
       </c>
       <c r="D46" s="1">
-        <v>43619.38875</v>
+        <v>43619.51375</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -24496,10 +24878,10 @@
         <v>233326486</v>
       </c>
       <c r="C47" s="1">
-        <v>43594.36887731482</v>
+        <v>43594.49387731482</v>
       </c>
       <c r="D47" s="1">
-        <v>43628.41805555556</v>
+        <v>43628.54305555556</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -25059,10 +25441,10 @@
         <v>233318351</v>
       </c>
       <c r="C48" s="1">
-        <v>43594.27174768518</v>
+        <v>43594.39674768518</v>
       </c>
       <c r="D48" s="1">
-        <v>43628.197592592594</v>
+        <v>43628.322592592594</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -25644,10 +26026,10 @@
         <v>233158854</v>
       </c>
       <c r="C49" s="1">
-        <v>43593.47342592593</v>
+        <v>43593.59842592593</v>
       </c>
       <c r="D49" s="1">
-        <v>43628.56653935185</v>
+        <v>43628.69153935185</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -26374,10 +26756,10 @@
         <v>231929806</v>
       </c>
       <c r="C50" s="1">
-        <v>43581.388773148145</v>
+        <v>43581.513773148145</v>
       </c>
       <c r="D50" s="1">
-        <v>43628.2221875</v>
+        <v>43628.3471875</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -26774,10 +27156,10 @@
         <v>228637564</v>
       </c>
       <c r="C51" s="1">
-        <v>43556.49988425926</v>
+        <v>43556.62488425926</v>
       </c>
       <c r="D51" s="1">
-        <v>43628.70988425926</v>
+        <v>43628.83488425926</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -27254,10 +27636,10 @@
         <v>228637564</v>
       </c>
       <c r="C52" s="1">
-        <v>43556.35381944444</v>
+        <v>43556.47881944444</v>
       </c>
       <c r="D52" s="1">
-        <v>43628.51689814815</v>
+        <v>43628.64189814815</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -28044,10 +28426,10 @@
         <v>228637564</v>
       </c>
       <c r="C53" s="1">
-        <v>43552.51997685185</v>
+        <v>43552.64497685185</v>
       </c>
       <c r="D53" s="1">
-        <v>43692.390555555554</v>
+        <v>43692.515555555554</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -28535,10 +28917,10 @@
         <v>226101601</v>
       </c>
       <c r="C54" s="1">
-        <v>43520.390914351854</v>
+        <v>43520.515914351854</v>
       </c>
       <c r="D54" s="1">
-        <v>43739.358877314815</v>
+        <v>43739.483877314815</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -29039,10 +29421,10 @@
         <v>226208327</v>
       </c>
       <c r="C55" s="1">
-        <v>43518.48881944444</v>
+        <v>43518.61381944444</v>
       </c>
       <c r="D55" s="1">
-        <v>43655.5522337963</v>
+        <v>43655.6772337963</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>

</xml_diff>